<commit_message>
Reworked making E directly from input rather than using many functions
</commit_message>
<xml_diff>
--- a/inst/extdata/example2-with-sims.xlsx
+++ b/inst/extdata/example2-with-sims.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DF2BE8-2CE4-7847-A242-5A5A63D0394E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806DF80D-6811-B546-8415-4D2CFF70057C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="760" windowWidth="28860" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="760" windowWidth="28860" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="11" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="140">
   <si>
     <t>trunc_pdf</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t>redd_activity</t>
+  </si>
+  <si>
+    <t>round_digits</t>
   </si>
 </sst>
 </file>
@@ -2106,51 +2109,51 @@
       </c>
       <c r="B14" s="84">
         <f t="shared" ref="B14:M14" ca="1" si="0">MEDIAN(_xlfn.ANCHORARRAY(B20))</f>
-        <v>21732.5</v>
+        <v>21640.5</v>
       </c>
       <c r="C14" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>11672</v>
+        <v>10820</v>
       </c>
       <c r="D14" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>57795</v>
+        <v>44513</v>
       </c>
       <c r="E14" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>16884</v>
+        <v>17368</v>
       </c>
       <c r="F14" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>312948</v>
+        <v>306375.5</v>
       </c>
       <c r="G14" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>22836</v>
+        <v>22113</v>
       </c>
       <c r="H14" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>2178</v>
+        <v>1870</v>
       </c>
       <c r="I14" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>1826</v>
+        <v>2530</v>
       </c>
       <c r="J14" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>6495</v>
+        <v>5963.5</v>
       </c>
       <c r="K14" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>6785</v>
+        <v>5845</v>
       </c>
       <c r="L14" s="85">
         <f t="shared" ca="1" si="0"/>
-        <v>46156</v>
+        <v>45583.5</v>
       </c>
       <c r="M14" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>5644</v>
+        <v>5614.5</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2159,51 +2162,51 @@
       </c>
       <c r="B15" s="87">
         <f t="shared" ref="B15:M15" ca="1" si="1">ROUND(B16/B14,2)</f>
-        <v>0.69</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C15" s="88">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21</v>
+        <v>0.6</v>
       </c>
       <c r="D15" s="88">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35</v>
+        <v>0.47</v>
       </c>
       <c r="E15" s="88">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
       <c r="F15" s="88">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16</v>
+        <v>0.09</v>
       </c>
       <c r="G15" s="88">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="H15" s="88">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24</v>
+        <v>0.35</v>
       </c>
       <c r="I15" s="88">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23</v>
+        <v>0.36</v>
       </c>
       <c r="J15" s="88">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
       <c r="K15" s="88">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
       <c r="L15" s="88">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M15" s="89">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2212,51 +2215,51 @@
       </c>
       <c r="B16" s="90">
         <f t="shared" ref="B16:M16" ca="1" si="2">(B18-B17)/2</f>
-        <v>14902.650000000001</v>
+        <v>6318.5499999999993</v>
       </c>
       <c r="C16" s="91">
         <f t="shared" ca="1" si="2"/>
-        <v>2430.5</v>
+        <v>6524.6749999999993</v>
       </c>
       <c r="D16" s="91">
         <f t="shared" ca="1" si="2"/>
-        <v>20340.650000000001</v>
+        <v>20988.424999999996</v>
       </c>
       <c r="E16" s="91">
         <f t="shared" ca="1" si="2"/>
-        <v>5099.4250000000002</v>
+        <v>4714.4500000000007</v>
       </c>
       <c r="F16" s="91">
         <f t="shared" ca="1" si="2"/>
-        <v>49590.875</v>
+        <v>26833.324999999983</v>
       </c>
       <c r="G16" s="91">
         <f t="shared" ca="1" si="2"/>
-        <v>2921.7250000000004</v>
+        <v>2240.625</v>
       </c>
       <c r="H16" s="91">
         <f t="shared" ca="1" si="2"/>
-        <v>533.25</v>
+        <v>659.35</v>
       </c>
       <c r="I16" s="91">
         <f t="shared" ca="1" si="2"/>
-        <v>420.44999999999993</v>
+        <v>909.35000000000014</v>
       </c>
       <c r="J16" s="91">
         <f t="shared" ca="1" si="2"/>
-        <v>1718.1749999999997</v>
+        <v>1261.9499999999998</v>
       </c>
       <c r="K16" s="91">
         <f t="shared" ca="1" si="2"/>
-        <v>2209.9</v>
+        <v>1982.7750000000001</v>
       </c>
       <c r="L16" s="91">
         <f t="shared" ca="1" si="2"/>
-        <v>3136.3250000000007</v>
+        <v>6275.2750000000015</v>
       </c>
       <c r="M16" s="92">
         <f t="shared" ca="1" si="2"/>
-        <v>538.94999999999982</v>
+        <v>1058.1500000000001</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2265,51 +2268,51 @@
       </c>
       <c r="B17" s="90">
         <f t="shared" ref="B17:M17" ca="1" si="3">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(B20),ci_alpha/2),2)</f>
-        <v>3511.85</v>
+        <v>13030.95</v>
       </c>
       <c r="C17" s="91">
         <f t="shared" ca="1" si="3"/>
-        <v>8695.35</v>
+        <v>5265.95</v>
       </c>
       <c r="D17" s="91">
         <f t="shared" ca="1" si="3"/>
-        <v>30410.2</v>
+        <v>29176.799999999999</v>
       </c>
       <c r="E17" s="91">
         <f t="shared" ca="1" si="3"/>
-        <v>12819.9</v>
+        <v>12154.8</v>
       </c>
       <c r="F17" s="91">
         <f t="shared" ca="1" si="3"/>
-        <v>273653.75</v>
+        <v>287474.95</v>
       </c>
       <c r="G17" s="91">
         <f t="shared" ca="1" si="3"/>
-        <v>19615.55</v>
+        <v>21057.65</v>
       </c>
       <c r="H17" s="91">
         <f t="shared" ca="1" si="3"/>
-        <v>1486.15</v>
+        <v>1409.95</v>
       </c>
       <c r="I17" s="91">
         <f t="shared" ca="1" si="3"/>
-        <v>1436.05</v>
+        <v>1579.35</v>
       </c>
       <c r="J17" s="91">
         <f t="shared" ca="1" si="3"/>
-        <v>5146.7</v>
+        <v>4660.5</v>
       </c>
       <c r="K17" s="91">
         <f t="shared" ca="1" si="3"/>
-        <v>3860.2</v>
+        <v>3267</v>
       </c>
       <c r="L17" s="91">
         <f t="shared" ca="1" si="3"/>
-        <v>42213.65</v>
+        <v>39690.75</v>
       </c>
       <c r="M17" s="92">
         <f t="shared" ca="1" si="3"/>
-        <v>5217.8500000000004</v>
+        <v>4280.95</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2318,51 +2321,51 @@
       </c>
       <c r="B18" s="90">
         <f t="shared" ref="B18:M18" ca="1" si="4">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(B20), 1 - ci_alpha / 2), 2)</f>
-        <v>33317.15</v>
+        <v>25668.05</v>
       </c>
       <c r="C18" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>13556.35</v>
+        <v>18315.3</v>
       </c>
       <c r="D18" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>71091.5</v>
+        <v>71153.649999999994</v>
       </c>
       <c r="E18" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>23018.75</v>
+        <v>21583.7</v>
       </c>
       <c r="F18" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>372835.5</v>
+        <v>341141.6</v>
       </c>
       <c r="G18" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>25459</v>
+        <v>25538.9</v>
       </c>
       <c r="H18" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>2552.65</v>
+        <v>2728.65</v>
       </c>
       <c r="I18" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>2276.9499999999998</v>
+        <v>3398.05</v>
       </c>
       <c r="J18" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>8583.0499999999993</v>
+        <v>7184.4</v>
       </c>
       <c r="K18" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>8280</v>
+        <v>7232.55</v>
       </c>
       <c r="L18" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>48486.3</v>
+        <v>52241.3</v>
       </c>
       <c r="M18" s="92">
         <f t="shared" ca="1" si="4"/>
-        <v>6295.75</v>
+        <v>6397.25</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2387,51 +2390,51 @@
       </c>
       <c r="B20" s="94" cm="1">
         <f t="array" aca="1" ref="B20:B29" ca="1">IF(B12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),B6,B7),0),_xlfn.SEQUENCE(n_iter, 1, B6, 0))</f>
-        <v>27788</v>
+        <v>25618</v>
       </c>
       <c r="C20" s="95" cm="1">
         <f t="array" aca="1" ref="C20:C29" ca="1">IF(C12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),C6,C7),0),_xlfn.SEQUENCE(n_iter, 1, C6, 0))</f>
-        <v>11822</v>
+        <v>16178</v>
       </c>
       <c r="D20" s="95" cm="1">
         <f t="array" aca="1" ref="D20:D29" ca="1">IF(D12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),D6,D7),0),_xlfn.SEQUENCE(n_iter, 1, D6, 0))</f>
-        <v>68721</v>
+        <v>56612</v>
       </c>
       <c r="E20" s="95" cm="1">
         <f t="array" aca="1" ref="E20:E29" ca="1">IF(E12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),E6,E7),0),_xlfn.SEQUENCE(n_iter, 1, E6, 0))</f>
-        <v>22235</v>
+        <v>10263</v>
       </c>
       <c r="F20" s="95" cm="1">
         <f t="array" aca="1" ref="F20:F29" ca="1">IF(F12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),F6,F7),0),_xlfn.SEQUENCE(n_iter, 1, F6, 0))</f>
-        <v>274003</v>
+        <v>318552</v>
       </c>
       <c r="G20" s="95" cm="1">
         <f t="array" aca="1" ref="G20:G29" ca="1">IF(G12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),G6,G7),0),_xlfn.SEQUENCE(n_iter, 1, G6, 0))</f>
-        <v>22640</v>
+        <v>21423</v>
       </c>
       <c r="H20" s="95" cm="1">
         <f t="array" aca="1" ref="H20:H29" ca="1">IF(H12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),H6,H7),0),_xlfn.SEQUENCE(n_iter, 1, H6, 0))</f>
-        <v>2180</v>
+        <v>1849</v>
       </c>
       <c r="I20" s="95" cm="1">
         <f t="array" aca="1" ref="I20:I29" ca="1">IF(I12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),I6,I7),0),_xlfn.SEQUENCE(n_iter, 1, I6, 0))</f>
-        <v>2299</v>
+        <v>1664</v>
       </c>
       <c r="J20" s="95" cm="1">
         <f t="array" aca="1" ref="J20:J29" ca="1">IF(J12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),J6,J7),0),_xlfn.SEQUENCE(n_iter, 1, J6, 0))</f>
-        <v>6557</v>
+        <v>6230</v>
       </c>
       <c r="K20" s="95" cm="1">
         <f t="array" aca="1" ref="K20:K29" ca="1">IF(K12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),K6,K7),0),_xlfn.SEQUENCE(n_iter, 1, K6, 0))</f>
-        <v>6890</v>
+        <v>4379</v>
       </c>
       <c r="L20" s="95" cm="1">
         <f t="array" aca="1" ref="L20:L29" ca="1">IF(L12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),L6,L7),0),_xlfn.SEQUENCE(n_iter, 1, L6, 0))</f>
-        <v>47528</v>
+        <v>40128</v>
       </c>
       <c r="M20" s="95" cm="1">
         <f t="array" aca="1" ref="M20:M29" ca="1">IF(M12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),M6,M7),0),_xlfn.SEQUENCE(n_iter, 1, M6, 0))</f>
-        <v>5434</v>
+        <v>5487</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2440,51 +2443,51 @@
       </c>
       <c r="B21">
         <f ca="1"/>
-        <v>23807</v>
+        <v>21726</v>
       </c>
       <c r="C21">
         <f ca="1"/>
-        <v>11510</v>
+        <v>11697</v>
       </c>
       <c r="D21">
         <f ca="1"/>
-        <v>55599</v>
+        <v>40741</v>
       </c>
       <c r="E21">
         <f ca="1"/>
-        <v>11415</v>
+        <v>18914</v>
       </c>
       <c r="F21">
         <f ca="1"/>
-        <v>273368</v>
+        <v>299981</v>
       </c>
       <c r="G21">
         <f ca="1"/>
-        <v>24124</v>
+        <v>22334</v>
       </c>
       <c r="H21">
         <f ca="1"/>
-        <v>1688</v>
+        <v>1603</v>
       </c>
       <c r="I21">
         <f ca="1"/>
-        <v>1691</v>
+        <v>2747</v>
       </c>
       <c r="J21">
         <f ca="1"/>
-        <v>6084</v>
+        <v>4842</v>
       </c>
       <c r="K21">
         <f ca="1"/>
-        <v>7109</v>
+        <v>5977</v>
       </c>
       <c r="L21">
         <f ca="1"/>
-        <v>48016</v>
+        <v>44126</v>
       </c>
       <c r="M21">
         <f ca="1"/>
-        <v>5742</v>
+        <v>6312</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2493,51 +2496,51 @@
       </c>
       <c r="B22">
         <f ca="1"/>
-        <v>36014</v>
+        <v>18633</v>
       </c>
       <c r="C22">
         <f ca="1"/>
-        <v>13897</v>
+        <v>7071</v>
       </c>
       <c r="D22">
         <f ca="1"/>
-        <v>73031</v>
+        <v>61703</v>
       </c>
       <c r="E22">
         <f ca="1"/>
-        <v>14537</v>
+        <v>23120</v>
       </c>
       <c r="F22">
         <f ca="1"/>
-        <v>324593</v>
+        <v>347825</v>
       </c>
       <c r="G22">
         <f ca="1"/>
-        <v>21584</v>
+        <v>25144</v>
       </c>
       <c r="H22">
         <f ca="1"/>
-        <v>2441</v>
+        <v>1853</v>
       </c>
       <c r="I22">
         <f ca="1"/>
-        <v>1813</v>
+        <v>1542</v>
       </c>
       <c r="J22">
         <f ca="1"/>
-        <v>6498</v>
+        <v>6786</v>
       </c>
       <c r="K22">
         <f ca="1"/>
-        <v>6680</v>
+        <v>6869</v>
       </c>
       <c r="L22">
         <f ca="1"/>
-        <v>45455</v>
+        <v>45219</v>
       </c>
       <c r="M22">
         <f ca="1"/>
-        <v>6568</v>
+        <v>4738</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2546,51 +2549,51 @@
       </c>
       <c r="B23">
         <f ca="1"/>
-        <v>17485</v>
+        <v>19072</v>
       </c>
       <c r="C23">
         <f ca="1"/>
-        <v>10061</v>
+        <v>5180</v>
       </c>
       <c r="D23">
         <f ca="1"/>
-        <v>55190</v>
+        <v>39678</v>
       </c>
       <c r="E23">
         <f ca="1"/>
-        <v>16775</v>
+        <v>18432</v>
       </c>
       <c r="F23">
         <f ca="1"/>
-        <v>347654</v>
+        <v>295500</v>
       </c>
       <c r="G23">
         <f ca="1"/>
-        <v>22011</v>
+        <v>23054</v>
       </c>
       <c r="H23">
         <f ca="1"/>
-        <v>2258</v>
+        <v>2694</v>
       </c>
       <c r="I23">
         <f ca="1"/>
-        <v>2250</v>
+        <v>2004</v>
       </c>
       <c r="J23">
         <f ca="1"/>
-        <v>8456</v>
+        <v>5915</v>
       </c>
       <c r="K23">
         <f ca="1"/>
-        <v>6065</v>
+        <v>3597</v>
       </c>
       <c r="L23">
         <f ca="1"/>
-        <v>48120</v>
+        <v>46012</v>
       </c>
       <c r="M23">
         <f ca="1"/>
-        <v>5122</v>
+        <v>3979</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2599,51 +2602,51 @@
       </c>
       <c r="B24">
         <f ca="1"/>
-        <v>30021</v>
+        <v>18053</v>
       </c>
       <c r="C24">
         <f ca="1"/>
-        <v>7578</v>
+        <v>10295</v>
       </c>
       <c r="D24">
         <f ca="1"/>
-        <v>59991</v>
+        <v>53552</v>
       </c>
       <c r="E24">
         <f ca="1"/>
-        <v>15951</v>
+        <v>14467</v>
       </c>
       <c r="F24">
         <f ca="1"/>
-        <v>304630</v>
+        <v>309936</v>
       </c>
       <c r="G24">
         <f ca="1"/>
-        <v>18833</v>
+        <v>21892</v>
       </c>
       <c r="H24">
         <f ca="1"/>
-        <v>1689</v>
+        <v>1697</v>
       </c>
       <c r="I24">
         <f ca="1"/>
-        <v>1315</v>
+        <v>3160</v>
       </c>
       <c r="J24">
         <f ca="1"/>
-        <v>4550</v>
+        <v>6012</v>
       </c>
       <c r="K24">
         <f ca="1"/>
-        <v>7708</v>
+        <v>6062</v>
       </c>
       <c r="L24">
         <f ca="1"/>
-        <v>42443</v>
+        <v>56402</v>
       </c>
       <c r="M24">
         <f ca="1"/>
-        <v>5335</v>
+        <v>5762</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2652,51 +2655,51 @@
       </c>
       <c r="B25">
         <f ca="1"/>
-        <v>374</v>
+        <v>8922</v>
       </c>
       <c r="C25">
         <f ca="1"/>
-        <v>12889</v>
+        <v>9575</v>
       </c>
       <c r="D25">
         <f ca="1"/>
-        <v>46479</v>
+        <v>22848</v>
       </c>
       <c r="E25">
         <f ca="1"/>
-        <v>16993</v>
+        <v>16089</v>
       </c>
       <c r="F25">
         <f ca="1"/>
-        <v>359663</v>
+        <v>332973</v>
       </c>
       <c r="G25">
         <f ca="1"/>
-        <v>23032</v>
+        <v>20816</v>
       </c>
       <c r="H25">
         <f ca="1"/>
-        <v>2176</v>
+        <v>1887</v>
       </c>
       <c r="I25">
         <f ca="1"/>
-        <v>1623</v>
+        <v>2851</v>
       </c>
       <c r="J25">
         <f ca="1"/>
-        <v>6492</v>
+        <v>7136</v>
       </c>
       <c r="K25">
         <f ca="1"/>
-        <v>8748</v>
+        <v>4914</v>
       </c>
       <c r="L25">
         <f ca="1"/>
-        <v>42026</v>
+        <v>45982</v>
       </c>
       <c r="M25">
         <f ca="1"/>
-        <v>5612</v>
+        <v>6467</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2705,51 +2708,51 @@
       </c>
       <c r="B26">
         <f ca="1"/>
-        <v>7347</v>
+        <v>21555</v>
       </c>
       <c r="C26">
         <f ca="1"/>
-        <v>12590</v>
+        <v>12152</v>
       </c>
       <c r="D26">
         <f ca="1"/>
-        <v>68032</v>
+        <v>78886</v>
       </c>
       <c r="E26">
         <f ca="1"/>
-        <v>19640</v>
+        <v>16775</v>
       </c>
       <c r="F26">
         <f ca="1"/>
-        <v>290304</v>
+        <v>323838</v>
       </c>
       <c r="G26">
         <f ca="1"/>
-        <v>20572</v>
+        <v>21707</v>
       </c>
       <c r="H26">
         <f ca="1"/>
-        <v>1979</v>
+        <v>2152</v>
       </c>
       <c r="I26">
         <f ca="1"/>
-        <v>1839</v>
+        <v>1625</v>
       </c>
       <c r="J26">
         <f ca="1"/>
-        <v>6162</v>
+        <v>4943</v>
       </c>
       <c r="K26">
         <f ca="1"/>
-        <v>4771</v>
+        <v>6644</v>
       </c>
       <c r="L26">
         <f ca="1"/>
-        <v>43590</v>
+        <v>44889</v>
       </c>
       <c r="M26">
         <f ca="1"/>
-        <v>5963</v>
+        <v>5742</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2758,51 +2761,51 @@
       </c>
       <c r="B27">
         <f ca="1"/>
-        <v>14038</v>
+        <v>22072</v>
       </c>
       <c r="C27">
         <f ca="1"/>
-        <v>11522</v>
+        <v>11345</v>
       </c>
       <c r="D27">
         <f ca="1"/>
-        <v>49745</v>
+        <v>45154</v>
       </c>
       <c r="E27">
         <f ca="1"/>
-        <v>15157</v>
+        <v>17961</v>
       </c>
       <c r="F27">
         <f ca="1"/>
-        <v>383613</v>
+        <v>280909</v>
       </c>
       <c r="G27">
         <f ca="1"/>
-        <v>24733</v>
+        <v>21353</v>
       </c>
       <c r="H27">
         <f ca="1"/>
-        <v>2644</v>
+        <v>1252</v>
       </c>
       <c r="I27">
         <f ca="1"/>
-        <v>1851</v>
+        <v>2313</v>
       </c>
       <c r="J27">
         <f ca="1"/>
-        <v>5876</v>
+        <v>4831</v>
       </c>
       <c r="K27">
         <f ca="1"/>
-        <v>3115</v>
+        <v>2997</v>
       </c>
       <c r="L27">
         <f ca="1"/>
-        <v>48786</v>
+        <v>39333</v>
       </c>
       <c r="M27">
         <f ca="1"/>
-        <v>5602</v>
+        <v>5749</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2811,51 +2814,51 @@
       </c>
       <c r="B28">
         <f ca="1"/>
-        <v>19658</v>
+        <v>25709</v>
       </c>
       <c r="C28">
         <f ca="1"/>
-        <v>13140</v>
+        <v>5371</v>
       </c>
       <c r="D28">
         <f ca="1"/>
-        <v>64942</v>
+        <v>43872</v>
       </c>
       <c r="E28">
         <f ca="1"/>
-        <v>18763</v>
+        <v>19706</v>
       </c>
       <c r="F28">
         <f ca="1"/>
-        <v>274252</v>
+        <v>299929</v>
       </c>
       <c r="G28">
         <f ca="1"/>
-        <v>26053</v>
+        <v>25862</v>
       </c>
       <c r="H28">
         <f ca="1"/>
-        <v>2347</v>
+        <v>2757</v>
       </c>
       <c r="I28">
         <f ca="1"/>
-        <v>2079</v>
+        <v>3205</v>
       </c>
       <c r="J28">
         <f ca="1"/>
-        <v>8687</v>
+        <v>4521</v>
       </c>
       <c r="K28">
         <f ca="1"/>
-        <v>6309</v>
+        <v>5713</v>
       </c>
       <c r="L28">
         <f ca="1"/>
-        <v>46154</v>
+        <v>45948</v>
       </c>
       <c r="M28">
         <f ca="1"/>
-        <v>5676</v>
+        <v>5235</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2864,51 +2867,51 @@
       </c>
       <c r="B29">
         <f ca="1"/>
-        <v>27357</v>
+        <v>25350</v>
       </c>
       <c r="C29">
         <f ca="1"/>
-        <v>10509</v>
+        <v>20064</v>
       </c>
       <c r="D29">
         <f ca="1"/>
-        <v>17263</v>
+        <v>36912</v>
       </c>
       <c r="E29">
         <f ca="1"/>
-        <v>23660</v>
+        <v>14548</v>
       </c>
       <c r="F29">
         <f ca="1"/>
-        <v>321266</v>
+        <v>302815</v>
       </c>
       <c r="G29">
         <f ca="1"/>
-        <v>24173</v>
+        <v>24257</v>
       </c>
       <c r="H29">
         <f ca="1"/>
-        <v>1321</v>
+        <v>2044</v>
       </c>
       <c r="I29">
         <f ca="1"/>
-        <v>1584</v>
+        <v>3556</v>
       </c>
       <c r="J29">
         <f ca="1"/>
-        <v>7035</v>
+        <v>7224</v>
       </c>
       <c r="K29">
         <f ca="1"/>
-        <v>7313</v>
+        <v>7530</v>
       </c>
       <c r="L29">
         <f ca="1"/>
-        <v>46158</v>
+        <v>47156</v>
       </c>
       <c r="M29">
         <f ca="1"/>
-        <v>5871</v>
+        <v>4650</v>
       </c>
     </row>
   </sheetData>
@@ -3352,82 +3355,82 @@
       </c>
       <c r="B14" s="84">
         <f t="shared" ref="B14:W14" ca="1" si="0">MEDIAN(_xlfn.ANCHORARRAY(B20))</f>
-        <v>14026898</v>
+        <v>14574201.5</v>
       </c>
       <c r="C14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>5426681.5</v>
+        <v>5202001.5</v>
       </c>
       <c r="D14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>31401396</v>
+        <v>17947516.5</v>
       </c>
       <c r="E14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>6523698</v>
+        <v>7415531</v>
       </c>
       <c r="F14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>43728169.5</v>
+        <v>57399550.5</v>
       </c>
       <c r="G14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>2584538.5</v>
+        <v>2360804.5</v>
       </c>
       <c r="H14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>1333066.5</v>
+        <v>1303271</v>
       </c>
       <c r="I14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>870888.5</v>
+        <v>1213908.5</v>
       </c>
       <c r="J14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>3269087</v>
+        <v>2289339.5</v>
       </c>
       <c r="K14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>2218934</v>
+        <v>2117391</v>
       </c>
       <c r="L14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>7305498.5</v>
+        <v>8387043</v>
       </c>
       <c r="M14" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>631925.5</v>
+        <v>461660.5</v>
       </c>
       <c r="N14" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>11850801</v>
+        <v>9646344</v>
       </c>
       <c r="O14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>9283585.5</v>
+        <v>11750730.5</v>
       </c>
       <c r="P14" s="109"/>
       <c r="Q14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>3859794</v>
+        <v>3636542</v>
       </c>
       <c r="R14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>3876647.5</v>
+        <v>4500064.5</v>
       </c>
       <c r="S14" s="109"/>
       <c r="T14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>20309610.5</v>
+        <v>21361677.5</v>
       </c>
       <c r="U14" s="109">
         <f t="shared" ca="1" si="0"/>
-        <v>7536411</v>
+        <v>8423781.5</v>
       </c>
       <c r="V14" s="109"/>
       <c r="W14" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>12413375.5</v>
+        <v>13555723</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3436,7 +3439,7 @@
       </c>
       <c r="B15" s="87">
         <f t="shared" ref="B15:W15" ca="1" si="1">ROUND(B16/B14,2)</f>
-        <v>0.73</v>
+        <v>0.41</v>
       </c>
       <c r="C15" s="75">
         <f t="shared" ca="1" si="1"/>
@@ -3444,74 +3447,74 @@
       </c>
       <c r="D15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47</v>
+        <v>0.79</v>
       </c>
       <c r="E15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42</v>
+        <v>0.53</v>
       </c>
       <c r="F15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>1.19</v>
+        <v>0.84</v>
       </c>
       <c r="G15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72</v>
+        <v>0.61</v>
       </c>
       <c r="H15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26</v>
+        <v>0.41</v>
       </c>
       <c r="I15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="J15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32</v>
+        <v>0.44</v>
       </c>
       <c r="K15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44</v>
+        <v>0.47</v>
       </c>
       <c r="L15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>1.08</v>
+        <v>0.91</v>
       </c>
       <c r="M15" s="76">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67</v>
+        <v>0.62</v>
       </c>
       <c r="N15" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31</v>
+        <v>0.41</v>
       </c>
       <c r="O15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1299999999999999</v>
+        <v>0.81</v>
       </c>
       <c r="P15" s="75"/>
       <c r="Q15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
       <c r="R15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>1.05</v>
+        <v>0.84</v>
       </c>
       <c r="S15" s="75"/>
       <c r="T15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.45</v>
+        <v>0.54</v>
       </c>
       <c r="U15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52</v>
+        <v>0.53</v>
       </c>
       <c r="V15" s="75"/>
       <c r="W15" s="76">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3520,82 +3523,82 @@
       </c>
       <c r="B16" s="84">
         <f t="shared" ref="B16:W16" ca="1" si="2">(B18-B17)/2</f>
-        <v>10260025.925000001</v>
+        <v>5992173.75</v>
       </c>
       <c r="C16" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>2229258.5</v>
+        <v>2117818.5499999998</v>
       </c>
       <c r="D16" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>14681378.725</v>
+        <v>14244244.625000002</v>
       </c>
       <c r="E16" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>2710407.7250000001</v>
+        <v>3961695.2</v>
       </c>
       <c r="F16" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>51823082.350000001</v>
+        <v>48109315.825000003</v>
       </c>
       <c r="G16" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>1873697.15</v>
+        <v>1439216.4</v>
       </c>
       <c r="H16" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>347853.375</v>
+        <v>536393</v>
       </c>
       <c r="I16" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>365580.54999999993</v>
+        <v>542503.82499999995</v>
       </c>
       <c r="J16" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>1032991.5</v>
+        <v>1017547.2</v>
       </c>
       <c r="K16" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>974153.60000000009</v>
+        <v>994804.60000000009</v>
       </c>
       <c r="L16" s="109">
         <f t="shared" ca="1" si="2"/>
-        <v>7881039.4749999996</v>
+        <v>7617523.5499999998</v>
       </c>
       <c r="M16" s="110">
         <f t="shared" ca="1" si="2"/>
-        <v>422148.92500000005</v>
+        <v>288427.47500000003</v>
       </c>
       <c r="N16" s="90">
         <f t="shared" ca="1" si="2"/>
-        <v>3644453.8000000003</v>
+        <v>3930924.9999999995</v>
       </c>
       <c r="O16" s="111">
         <f t="shared" ca="1" si="2"/>
-        <v>10457840.1</v>
+        <v>9535753.5</v>
       </c>
       <c r="P16" s="111"/>
       <c r="Q16" s="111">
         <f t="shared" ca="1" si="2"/>
-        <v>807580.52499999991</v>
+        <v>861292.35000000009</v>
       </c>
       <c r="R16" s="111">
         <f ca="1">(R18-R17)/2</f>
-        <v>4051823.8000000003</v>
+        <v>3758089.2749999999</v>
       </c>
       <c r="S16" s="111"/>
       <c r="T16" s="111">
         <f t="shared" ca="1" si="2"/>
-        <v>9146761.75</v>
+        <v>11512800.450000001</v>
       </c>
       <c r="U16" s="111">
         <f t="shared" ca="1" si="2"/>
-        <v>3948210.5999999996</v>
+        <v>4472859.45</v>
       </c>
       <c r="V16" s="111"/>
       <c r="W16" s="112">
         <f t="shared" ca="1" si="2"/>
-        <v>5391592.1500000004</v>
+        <v>7728024.4249999998</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3604,82 +3607,82 @@
       </c>
       <c r="B17" s="84">
         <f t="shared" ref="B17:O17" ca="1" si="3">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(B20),ci_alpha/2),2)</f>
-        <v>2026186.65</v>
+        <v>5159983.25</v>
       </c>
       <c r="C17" s="109">
         <f t="shared" ca="1" si="3"/>
-        <v>3424718.2</v>
+        <v>3154254.95</v>
       </c>
       <c r="D17" s="109">
         <f t="shared" ca="1" si="3"/>
-        <v>12044651.699999999</v>
+        <v>8038220.9500000002</v>
       </c>
       <c r="E17" s="109">
         <f t="shared" ca="1" si="3"/>
-        <v>4362960.95</v>
+        <v>2748903.75</v>
       </c>
       <c r="F17" s="109">
         <f t="shared" ca="1" si="3"/>
-        <v>-9786245.0500000007</v>
+        <v>18854288.850000001</v>
       </c>
       <c r="G17" s="109">
         <f t="shared" ca="1" si="3"/>
-        <v>558025.69999999995</v>
+        <v>862299.1</v>
       </c>
       <c r="H17" s="109">
         <f t="shared" ca="1" si="3"/>
-        <v>939353.75</v>
+        <v>578349.9</v>
       </c>
       <c r="I17" s="109">
         <f t="shared" ca="1" si="3"/>
-        <v>551193.55000000005</v>
+        <v>768537.55</v>
       </c>
       <c r="J17" s="109">
         <f t="shared" ca="1" si="3"/>
-        <v>2390434.9500000002</v>
+        <v>1448447.35</v>
       </c>
       <c r="K17" s="109">
         <f t="shared" ca="1" si="3"/>
-        <v>1572090.4</v>
+        <v>1259549.5</v>
       </c>
       <c r="L17" s="109">
         <f t="shared" ca="1" si="3"/>
-        <v>-1467846.5</v>
+        <v>2790442.9</v>
       </c>
       <c r="M17" s="110">
         <f t="shared" ca="1" si="3"/>
-        <v>147062.54999999999</v>
+        <v>244350.1</v>
       </c>
       <c r="N17" s="90">
         <f t="shared" ca="1" si="3"/>
-        <v>6444301.7999999998</v>
+        <v>5132580.95</v>
       </c>
       <c r="O17" s="111">
         <f t="shared" ca="1" si="3"/>
-        <v>-1756371.25</v>
+        <v>4297252.7</v>
       </c>
       <c r="P17" s="111"/>
       <c r="Q17" s="111">
         <f ca="1">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(Q20),ci_alpha/2),2)</f>
-        <v>3236375.5</v>
+        <v>2464847.15</v>
       </c>
       <c r="R17" s="111">
         <f ca="1">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(R20),ci_alpha/2),2)</f>
-        <v>-586629.9</v>
+        <v>1674617.8</v>
       </c>
       <c r="S17" s="111"/>
       <c r="T17" s="111">
         <f ca="1">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(T20),ci_alpha/2),2)</f>
-        <v>11955733.35</v>
+        <v>10677366.550000001</v>
       </c>
       <c r="U17" s="111">
         <f ca="1">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(U20),ci_alpha/2),2)</f>
-        <v>3733002.65</v>
+        <v>4155869.35</v>
       </c>
       <c r="V17" s="111"/>
       <c r="W17" s="112">
         <f ca="1">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(W20),ci_alpha/2),2)</f>
-        <v>7836648.7000000002</v>
+        <v>6458554.9000000004</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3688,82 +3691,82 @@
       </c>
       <c r="B18" s="84">
         <f t="shared" ref="B18:O18" ca="1" si="4">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(B20), 1 - ci_alpha / 2), 2)</f>
-        <v>22546238.5</v>
+        <v>17144330.75</v>
       </c>
       <c r="C18" s="109">
         <f t="shared" ca="1" si="4"/>
-        <v>7883235.2000000002</v>
+        <v>7389892.0499999998</v>
       </c>
       <c r="D18" s="109">
         <f t="shared" ca="1" si="4"/>
-        <v>41407409.149999999</v>
+        <v>36526710.200000003</v>
       </c>
       <c r="E18" s="109">
         <f t="shared" ca="1" si="4"/>
-        <v>9783776.4000000004</v>
+        <v>10672294.15</v>
       </c>
       <c r="F18" s="109">
         <f t="shared" ca="1" si="4"/>
-        <v>93859919.650000006</v>
+        <v>115072920.5</v>
       </c>
       <c r="G18" s="109">
         <f t="shared" ca="1" si="4"/>
-        <v>4305420</v>
+        <v>3740731.9</v>
       </c>
       <c r="H18" s="109">
         <f t="shared" ca="1" si="4"/>
-        <v>1635060.5</v>
+        <v>1651135.9</v>
       </c>
       <c r="I18" s="109">
         <f t="shared" ca="1" si="4"/>
-        <v>1282354.6499999999</v>
+        <v>1853545.2</v>
       </c>
       <c r="J18" s="109">
         <f t="shared" ca="1" si="4"/>
-        <v>4456417.95</v>
+        <v>3483541.75</v>
       </c>
       <c r="K18" s="109">
         <f t="shared" ca="1" si="4"/>
-        <v>3520397.6</v>
+        <v>3249158.7</v>
       </c>
       <c r="L18" s="109">
         <f t="shared" ca="1" si="4"/>
-        <v>14294232.449999999</v>
+        <v>18025490</v>
       </c>
       <c r="M18" s="110">
         <f t="shared" ca="1" si="4"/>
-        <v>991360.4</v>
+        <v>821205.05</v>
       </c>
       <c r="N18" s="90">
         <f t="shared" ca="1" si="4"/>
-        <v>13733209.4</v>
+        <v>12994430.949999999</v>
       </c>
       <c r="O18" s="111">
         <f t="shared" ca="1" si="4"/>
-        <v>19159308.949999999</v>
+        <v>23368759.699999999</v>
       </c>
       <c r="P18" s="111"/>
       <c r="Q18" s="111">
         <f ca="1">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(Q20), 1 - ci_alpha / 2), 2)</f>
-        <v>4851536.55</v>
+        <v>4187431.85</v>
       </c>
       <c r="R18" s="111">
         <f ca="1">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(R20), 1 - ci_alpha / 2), 2)</f>
-        <v>7517017.7000000002</v>
+        <v>9190796.3499999996</v>
       </c>
       <c r="S18" s="111"/>
       <c r="T18" s="111">
         <f ca="1">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(T20), 1 - ci_alpha / 2), 2)</f>
-        <v>30249256.850000001</v>
+        <v>33702967.450000003</v>
       </c>
       <c r="U18" s="111">
         <f ca="1">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(U20), 1 - ci_alpha / 2), 2)</f>
-        <v>11629423.85</v>
+        <v>13101588.25</v>
       </c>
       <c r="V18" s="111"/>
       <c r="W18" s="112">
         <f ca="1">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(W20), 1 - ci_alpha / 2), 2)</f>
-        <v>18619833</v>
+        <v>21914603.75</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3782,7 +3785,7 @@
       <c r="M19" s="115"/>
       <c r="N19" s="116">
         <f ca="1">ROUND(SUM(B20:E20) / year_ref,0)</f>
-        <v>12592475</v>
+        <v>11954662</v>
       </c>
       <c r="O19" s="114"/>
       <c r="P19" s="54"/>
@@ -3801,82 +3804,82 @@
       </c>
       <c r="B20" s="126" cm="1">
         <f t="array" aca="1" ref="B20:B29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!B20) *_xlfn.ANCHORARRAY( SIMS_EF!B20), 0)</f>
-        <v>18317044</v>
+        <v>17646011</v>
       </c>
       <c r="C20" s="126" cm="1">
         <f t="array" aca="1" ref="C20:C29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!C20) *_xlfn.ANCHORARRAY( SIMS_EF!C20), 0)</f>
-        <v>4892097</v>
+        <v>7439712</v>
       </c>
       <c r="D20" s="126" cm="1">
         <f t="array" aca="1" ref="D20:D29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!D20) *_xlfn.ANCHORARRAY( SIMS_EF!D20), 0)</f>
-        <v>33340062</v>
+        <v>31313060</v>
       </c>
       <c r="E20" s="126" cm="1">
         <f t="array" aca="1" ref="E20:E29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!E20) *_xlfn.ANCHORARRAY( SIMS_EF!E20), 0)</f>
-        <v>6413174</v>
+        <v>3374526</v>
       </c>
       <c r="F20" s="126" cm="1">
         <f t="array" aca="1" ref="F20:F29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!F20) *_xlfn.ANCHORARRAY( SIMS_EF!F20), 0)</f>
-        <v>47682002</v>
+        <v>43226232</v>
       </c>
       <c r="G20" s="126" cm="1">
         <f t="array" aca="1" ref="G20:G29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!G20) *_xlfn.ANCHORARRAY( SIMS_EF!G20), 0)</f>
-        <v>2838716</v>
+        <v>2807720</v>
       </c>
       <c r="H20" s="126" cm="1">
         <f t="array" aca="1" ref="H20:H29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!H20) *_xlfn.ANCHORARRAY( SIMS_EF!H20), 0)</f>
-        <v>1436993</v>
+        <v>1273615</v>
       </c>
       <c r="I20" s="126" cm="1">
         <f t="array" aca="1" ref="I20:I29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!I20) *_xlfn.ANCHORARRAY( SIMS_EF!I20), 0)</f>
-        <v>951356</v>
+        <v>765217</v>
       </c>
       <c r="J20" s="126" cm="1">
         <f t="array" aca="1" ref="J20:J29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!J20) *_xlfn.ANCHORARRAY( SIMS_EF!J20), 0)</f>
-        <v>3181135</v>
+        <v>3445919</v>
       </c>
       <c r="K20" s="126" cm="1">
         <f t="array" aca="1" ref="K20:K29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!K20) *_xlfn.ANCHORARRAY( SIMS_EF!K20), 0)</f>
-        <v>1987262</v>
+        <v>1439837</v>
       </c>
       <c r="L20" s="126" cm="1">
         <f t="array" aca="1" ref="L20:L29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!L20) *_xlfn.ANCHORARRAY( SIMS_EF!L20), 0)</f>
-        <v>8270823</v>
+        <v>5445209</v>
       </c>
       <c r="M20" s="126" cm="1">
         <f t="array" aca="1" ref="M20:M29" ca="1">ROUND(_xlfn.ANCHORARRAY(SIMS_AD!M20) *_xlfn.ANCHORARRAY( SIMS_EF!M20), 0)</f>
-        <v>681342</v>
+        <v>719132</v>
       </c>
       <c r="N20" s="117" cm="1">
         <f t="array" aca="1" ref="N20:N29" ca="1">_xlfn.BYROW(_xlfn.ANCHORARRAY(B20):_xlfn.ANCHORARRAY(E20),_xlfn.LAMBDA(_xlpm.x, ROUND(SUM(_xlpm.x)/year_ref,0)))</f>
-        <v>12592475</v>
+        <v>11954662</v>
       </c>
       <c r="O20" s="117" cm="1">
         <f t="array" aca="1" ref="O20:O29" ca="1">_xlfn.BYROW(_xlfn.ANCHORARRAY(F20):_xlfn.ANCHORARRAY(G20),_xlfn.LAMBDA(_xlpm.x, ROUND(SUM(_xlpm.x)/year_ref,0)))</f>
-        <v>10104144</v>
+        <v>9206790</v>
       </c>
       <c r="P20" s="118"/>
       <c r="Q20" s="117" cm="1">
         <f t="array" aca="1" ref="Q20:Q29" ca="1">_xlfn.BYROW(_xlfn.ANCHORARRAY(H20):_xlfn.ANCHORARRAY(K20),_xlfn.LAMBDA(_xlpm.x, ROUND(SUM(_xlpm.x)/year_mon,0)))</f>
-        <v>3778373</v>
+        <v>3462294</v>
       </c>
       <c r="R20" s="117" cm="1">
         <f t="array" aca="1" ref="R20:R29" ca="1">_xlfn.BYROW(_xlfn.ANCHORARRAY(L20):_xlfn.ANCHORARRAY(M20),_xlfn.LAMBDA(_xlpm.x, ROUND(SUM(_xlpm.x)/year_mon,0)))</f>
-        <v>4476083</v>
+        <v>3082171</v>
       </c>
       <c r="S20" s="118"/>
       <c r="T20" s="117" cm="1">
         <f t="array" aca="1" ref="T20:T29" ca="1">_xlfn.ANCHORARRAY(N20) +_xlfn.ANCHORARRAY( O20)</f>
-        <v>22696619</v>
+        <v>21161452</v>
       </c>
       <c r="U20" s="117" cm="1">
         <f t="array" aca="1" ref="U20:U29" ca="1">_xlfn.ANCHORARRAY(Q20) +_xlfn.ANCHORARRAY( R20)</f>
-        <v>8254456</v>
+        <v>6544465</v>
       </c>
       <c r="V20" s="118"/>
       <c r="W20" s="117" cm="1">
         <f t="array" aca="1" ref="W20:W29" ca="1">_xlfn.ANCHORARRAY(T20) -_xlfn.ANCHORARRAY( U20)</f>
-        <v>14442163</v>
+        <v>14616987</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3885,79 +3888,79 @@
       </c>
       <c r="B21">
         <f ca="1"/>
-        <v>21412540</v>
+        <v>14048792</v>
       </c>
       <c r="C21">
         <f ca="1"/>
-        <v>7007864</v>
+        <v>7329001</v>
       </c>
       <c r="D21">
         <f ca="1"/>
-        <v>30804292</v>
+        <v>17018534</v>
       </c>
       <c r="E21">
         <f ca="1"/>
-        <v>5664283</v>
+        <v>10808065</v>
       </c>
       <c r="F21">
         <f ca="1"/>
-        <v>94415293</v>
+        <v>68668651</v>
       </c>
       <c r="G21">
         <f ca="1"/>
-        <v>2717231</v>
+        <v>1231474</v>
       </c>
       <c r="H21">
         <f ca="1"/>
-        <v>1518224</v>
+        <v>1036556</v>
       </c>
       <c r="I21">
         <f ca="1"/>
-        <v>1029565</v>
+        <v>1721191</v>
       </c>
       <c r="J21">
         <f ca="1"/>
-        <v>3370804</v>
+        <v>2022624</v>
       </c>
       <c r="K21">
         <f ca="1"/>
-        <v>3527585</v>
+        <v>3415449</v>
       </c>
       <c r="L21">
         <f ca="1"/>
-        <v>16583670</v>
+        <v>10100883</v>
       </c>
       <c r="M21">
         <f ca="1"/>
-        <v>646756</v>
+        <v>348037</v>
       </c>
       <c r="N21">
         <f ca="1"/>
-        <v>12977796</v>
+        <v>9840878</v>
       </c>
       <c r="O21">
         <f ca="1"/>
-        <v>19426505</v>
+        <v>13980025</v>
       </c>
       <c r="Q21">
         <f ca="1"/>
-        <v>4723089</v>
+        <v>4097910</v>
       </c>
       <c r="R21">
         <f ca="1"/>
-        <v>8615213</v>
+        <v>5224460</v>
       </c>
       <c r="T21">
         <f ca="1"/>
-        <v>32404301</v>
+        <v>23820903</v>
       </c>
       <c r="U21">
         <f ca="1"/>
-        <v>13338302</v>
+        <v>9322370</v>
       </c>
       <c r="W21">
         <f ca="1"/>
-        <v>19065999</v>
+        <v>14498533</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3966,79 +3969,79 @@
       </c>
       <c r="B22">
         <f ca="1"/>
-        <v>19312652</v>
+        <v>14211315</v>
       </c>
       <c r="C22">
         <f ca="1"/>
-        <v>5349219</v>
+        <v>3542818</v>
       </c>
       <c r="D22">
         <f ca="1"/>
-        <v>39241601</v>
+        <v>26024413</v>
       </c>
       <c r="E22">
         <f ca="1"/>
-        <v>5237434</v>
+        <v>9452473</v>
       </c>
       <c r="F22">
         <f ca="1"/>
-        <v>-348613</v>
+        <v>118582934</v>
       </c>
       <c r="G22">
         <f ca="1"/>
-        <v>531743</v>
+        <v>2318051</v>
       </c>
       <c r="H22">
         <f ca="1"/>
-        <v>1308996</v>
+        <v>1413276</v>
       </c>
       <c r="I22">
         <f ca="1"/>
-        <v>697858</v>
+        <v>772596</v>
       </c>
       <c r="J22">
         <f ca="1"/>
-        <v>3491557</v>
+        <v>2862124</v>
       </c>
       <c r="K22">
         <f ca="1"/>
-        <v>2406690</v>
+        <v>2808349</v>
       </c>
       <c r="L22">
         <f ca="1"/>
-        <v>-48819</v>
+        <v>15416378</v>
       </c>
       <c r="M22">
         <f ca="1"/>
-        <v>161809</v>
+        <v>436801</v>
       </c>
       <c r="N22">
         <f ca="1"/>
-        <v>13828181</v>
+        <v>10646204</v>
       </c>
       <c r="O22">
         <f ca="1"/>
-        <v>36626</v>
+        <v>24180197</v>
       </c>
       <c r="Q22">
         <f ca="1"/>
-        <v>3952551</v>
+        <v>3928173</v>
       </c>
       <c r="R22">
         <f ca="1"/>
-        <v>56495</v>
+        <v>7926590</v>
       </c>
       <c r="T22">
         <f ca="1"/>
-        <v>13864807</v>
+        <v>34826401</v>
       </c>
       <c r="U22">
         <f ca="1"/>
-        <v>4009046</v>
+        <v>11854763</v>
       </c>
       <c r="W22">
         <f ca="1"/>
-        <v>9855761</v>
+        <v>22971638</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4047,79 +4050,79 @@
       </c>
       <c r="B23">
         <f ca="1"/>
-        <v>11612348</v>
+        <v>7307971</v>
       </c>
       <c r="C23">
         <f ca="1"/>
-        <v>5830148</v>
+        <v>3045089</v>
       </c>
       <c r="D23">
         <f ca="1"/>
-        <v>31998500</v>
+        <v>12862417</v>
       </c>
       <c r="E23">
         <f ca="1"/>
-        <v>6104641</v>
+        <v>8581607</v>
       </c>
       <c r="F23">
         <f ca="1"/>
-        <v>29322529</v>
+        <v>17436864</v>
       </c>
       <c r="G23">
         <f ca="1"/>
-        <v>4744845</v>
+        <v>2818859</v>
       </c>
       <c r="H23">
         <f ca="1"/>
-        <v>1499610</v>
+        <v>1032282</v>
       </c>
       <c r="I23">
         <f ca="1"/>
-        <v>1303830</v>
+        <v>1178061</v>
       </c>
       <c r="J23">
         <f ca="1"/>
-        <v>4902687</v>
+        <v>1917466</v>
       </c>
       <c r="K23">
         <f ca="1"/>
-        <v>2207132</v>
+        <v>1674698</v>
       </c>
       <c r="L23">
         <f ca="1"/>
-        <v>4058633</v>
+        <v>2715076</v>
       </c>
       <c r="M23">
         <f ca="1"/>
-        <v>1104134</v>
+        <v>486520</v>
       </c>
       <c r="N23">
         <f ca="1"/>
-        <v>11109127</v>
+        <v>6359417</v>
       </c>
       <c r="O23">
         <f ca="1"/>
-        <v>6813475</v>
+        <v>4051145</v>
       </c>
       <c r="Q23">
         <f ca="1"/>
-        <v>4956630</v>
+        <v>2901254</v>
       </c>
       <c r="R23">
         <f ca="1"/>
-        <v>2581384</v>
+        <v>1600798</v>
       </c>
       <c r="T23">
         <f ca="1"/>
-        <v>17922602</v>
+        <v>10410562</v>
       </c>
       <c r="U23">
         <f ca="1"/>
-        <v>7538014</v>
+        <v>4502052</v>
       </c>
       <c r="W23">
         <f ca="1"/>
-        <v>10384588</v>
+        <v>5908510</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4128,79 +4131,79 @@
       </c>
       <c r="B24">
         <f ca="1"/>
-        <v>23473810</v>
+        <v>14937088</v>
       </c>
       <c r="C24">
         <f ca="1"/>
-        <v>2790409</v>
+        <v>4318938</v>
       </c>
       <c r="D24">
         <f ca="1"/>
-        <v>35509033</v>
+        <v>25167512</v>
       </c>
       <c r="E24">
         <f ca="1"/>
-        <v>3647483</v>
+        <v>5340855</v>
       </c>
       <c r="F24">
         <f ca="1"/>
-        <v>57881832</v>
+        <v>110782904</v>
       </c>
       <c r="G24">
         <f ca="1"/>
-        <v>2628277</v>
+        <v>1102109</v>
       </c>
       <c r="H24">
         <f ca="1"/>
-        <v>1320651</v>
+        <v>1404101</v>
       </c>
       <c r="I24">
         <f ca="1"/>
-        <v>484216</v>
+        <v>1325677</v>
       </c>
       <c r="J24">
         <f ca="1"/>
-        <v>2693172</v>
+        <v>2825424</v>
       </c>
       <c r="K24">
         <f ca="1"/>
-        <v>1762573</v>
+        <v>2237939</v>
       </c>
       <c r="L24">
         <f ca="1"/>
-        <v>8064467</v>
+        <v>20160218</v>
       </c>
       <c r="M24">
         <f ca="1"/>
-        <v>744537</v>
+        <v>290076</v>
       </c>
       <c r="N24">
         <f ca="1"/>
-        <v>13084147</v>
+        <v>9952879</v>
       </c>
       <c r="O24">
         <f ca="1"/>
-        <v>12102022</v>
+        <v>22377003</v>
       </c>
       <c r="Q24">
         <f ca="1"/>
-        <v>3130306</v>
+        <v>3896571</v>
       </c>
       <c r="R24">
         <f ca="1"/>
-        <v>4404502</v>
+        <v>10225147</v>
       </c>
       <c r="T24">
         <f ca="1"/>
-        <v>25186169</v>
+        <v>32329882</v>
       </c>
       <c r="U24">
         <f ca="1"/>
-        <v>7534808</v>
+        <v>14121718</v>
       </c>
       <c r="W24">
         <f ca="1"/>
-        <v>17651361</v>
+        <v>18208164</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4209,79 +4212,79 @@
       </c>
       <c r="B25">
         <f ca="1"/>
-        <v>231255</v>
+        <v>3867446</v>
       </c>
       <c r="C25">
         <f ca="1"/>
-        <v>5504144</v>
+        <v>4197268</v>
       </c>
       <c r="D25">
         <f ca="1"/>
-        <v>16697534</v>
+        <v>6041422</v>
       </c>
       <c r="E25">
         <f ca="1"/>
-        <v>6821313</v>
+        <v>6537894</v>
       </c>
       <c r="F25">
         <f ca="1"/>
-        <v>93181130</v>
+        <v>56290751</v>
       </c>
       <c r="G25">
         <f ca="1"/>
-        <v>590149</v>
+        <v>666091</v>
       </c>
       <c r="H25">
         <f ca="1"/>
-        <v>1345482</v>
+        <v>817964</v>
       </c>
       <c r="I25">
         <f ca="1"/>
-        <v>693089</v>
+        <v>1249756</v>
       </c>
       <c r="J25">
         <f ca="1"/>
-        <v>2332245</v>
+        <v>1886887</v>
       </c>
       <c r="K25">
         <f ca="1"/>
-        <v>3511613</v>
+        <v>1996843</v>
       </c>
       <c r="L25">
         <f ca="1"/>
-        <v>10888054</v>
+        <v>7773487</v>
       </c>
       <c r="M25">
         <f ca="1"/>
-        <v>143796</v>
+        <v>206938</v>
       </c>
       <c r="N25">
         <f ca="1"/>
-        <v>5850849</v>
+        <v>4128806</v>
       </c>
       <c r="O25">
         <f ca="1"/>
-        <v>18754256</v>
+        <v>11391368</v>
       </c>
       <c r="Q25">
         <f ca="1"/>
-        <v>3941215</v>
+        <v>2975725</v>
       </c>
       <c r="R25">
         <f ca="1"/>
-        <v>5515925</v>
+        <v>3990213</v>
       </c>
       <c r="T25">
         <f ca="1"/>
-        <v>24605105</v>
+        <v>15520174</v>
       </c>
       <c r="U25">
         <f ca="1"/>
-        <v>9457140</v>
+        <v>6965938</v>
       </c>
       <c r="W25">
         <f ca="1"/>
-        <v>15147965</v>
+        <v>8554236</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4290,79 +4293,79 @@
       </c>
       <c r="B26">
         <f ca="1"/>
-        <v>4219992</v>
+        <v>16367444</v>
       </c>
       <c r="C26">
         <f ca="1"/>
-        <v>8599448</v>
+        <v>6085065</v>
       </c>
       <c r="D26">
         <f ca="1"/>
-        <v>43179434</v>
+        <v>40792424</v>
       </c>
       <c r="E26">
         <f ca="1"/>
-        <v>12086790</v>
+        <v>5980824</v>
       </c>
       <c r="F26">
         <f ca="1"/>
-        <v>-17507944</v>
+        <v>78442307</v>
       </c>
       <c r="G26">
         <f ca="1"/>
-        <v>1391099</v>
+        <v>3130453</v>
       </c>
       <c r="H26">
         <f ca="1"/>
-        <v>1136704</v>
+        <v>1634087</v>
       </c>
       <c r="I26">
         <f ca="1"/>
-        <v>1256107</v>
+        <v>813712</v>
       </c>
       <c r="J26">
         <f ca="1"/>
-        <v>3910978</v>
+        <v>2556055</v>
       </c>
       <c r="K26">
         <f ca="1"/>
-        <v>2936155</v>
+        <v>2368799</v>
       </c>
       <c r="L26">
         <f ca="1"/>
-        <v>-2628869</v>
+        <v>10873328</v>
       </c>
       <c r="M26">
         <f ca="1"/>
-        <v>403224</v>
+        <v>828077</v>
       </c>
       <c r="N26">
         <f ca="1"/>
-        <v>13617133</v>
+        <v>13845151</v>
       </c>
       <c r="O26">
         <f ca="1"/>
-        <v>-3223369</v>
+        <v>16314552</v>
       </c>
       <c r="Q26">
         <f ca="1"/>
-        <v>4619972</v>
+        <v>3686327</v>
       </c>
       <c r="R26">
         <f ca="1"/>
-        <v>-1112823</v>
+        <v>5850703</v>
       </c>
       <c r="T26">
         <f ca="1"/>
-        <v>10393764</v>
+        <v>30159703</v>
       </c>
       <c r="U26">
         <f ca="1"/>
-        <v>3507149</v>
+        <v>9537030</v>
       </c>
       <c r="W26">
         <f ca="1"/>
-        <v>6886615</v>
+        <v>20622673</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4371,79 +4374,79 @@
       </c>
       <c r="B27">
         <f ca="1"/>
-        <v>9188699</v>
+        <v>6739751</v>
       </c>
       <c r="C27">
         <f ca="1"/>
-        <v>6994004</v>
+        <v>6515377</v>
       </c>
       <c r="D27">
         <f ca="1"/>
-        <v>20839026</v>
+        <v>10478753</v>
       </c>
       <c r="E27">
         <f ca="1"/>
-        <v>6891160</v>
+        <v>8293168</v>
       </c>
       <c r="F27">
         <f ca="1"/>
-        <v>90395335</v>
+        <v>20586697</v>
       </c>
       <c r="G27">
         <f ca="1"/>
-        <v>3768345</v>
+        <v>2403558</v>
       </c>
       <c r="H27">
         <f ca="1"/>
-        <v>1730654</v>
+        <v>382302</v>
       </c>
       <c r="I27">
         <f ca="1"/>
-        <v>1123581</v>
+        <v>1328344</v>
       </c>
       <c r="J27">
         <f ca="1"/>
-        <v>2461556</v>
+        <v>1121116</v>
       </c>
       <c r="K27">
         <f ca="1"/>
-        <v>1416241</v>
+        <v>1383811</v>
       </c>
       <c r="L27">
         <f ca="1"/>
-        <v>11496031</v>
+        <v>2882558</v>
       </c>
       <c r="M27">
         <f ca="1"/>
-        <v>853526</v>
+        <v>647125</v>
       </c>
       <c r="N27">
         <f ca="1"/>
-        <v>8782578</v>
+        <v>6405410</v>
       </c>
       <c r="O27">
         <f ca="1"/>
-        <v>18832736</v>
+        <v>4598051</v>
       </c>
       <c r="Q27">
         <f ca="1"/>
-        <v>3366016</v>
+        <v>2107787</v>
       </c>
       <c r="R27">
         <f ca="1"/>
-        <v>6174779</v>
+        <v>1764842</v>
       </c>
       <c r="T27">
         <f ca="1"/>
-        <v>27615314</v>
+        <v>11003461</v>
       </c>
       <c r="U27">
         <f ca="1"/>
-        <v>9540795</v>
+        <v>3872629</v>
       </c>
       <c r="W27">
         <f ca="1"/>
-        <v>18074519</v>
+        <v>7130832</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4452,79 +4455,79 @@
       </c>
       <c r="B28">
         <f ca="1"/>
-        <v>9356697</v>
+        <v>15526899</v>
       </c>
       <c r="C28">
         <f ca="1"/>
-        <v>4995736</v>
+        <v>3287680</v>
       </c>
       <c r="D28">
         <f ca="1"/>
-        <v>21699200</v>
+        <v>17938120</v>
       </c>
       <c r="E28">
         <f ca="1"/>
-        <v>6634222</v>
+        <v>10506352</v>
       </c>
       <c r="F28">
         <f ca="1"/>
-        <v>38900178</v>
+        <v>58508350</v>
       </c>
       <c r="G28">
         <f ca="1"/>
-        <v>693348</v>
+        <v>2042115</v>
       </c>
       <c r="H28">
         <f ca="1"/>
-        <v>1117111</v>
+        <v>1665085</v>
       </c>
       <c r="I28">
         <f ca="1"/>
-        <v>790421</v>
+        <v>1961835</v>
       </c>
       <c r="J28">
         <f ca="1"/>
-        <v>2902605</v>
+        <v>1848519</v>
       </c>
       <c r="K28">
         <f ca="1"/>
-        <v>2230736</v>
+        <v>3045915</v>
       </c>
       <c r="L28">
         <f ca="1"/>
-        <v>6546530</v>
+        <v>8963260</v>
       </c>
       <c r="M28">
         <f ca="1"/>
-        <v>151055</v>
+        <v>413366</v>
       </c>
       <c r="N28">
         <f ca="1"/>
-        <v>8537171</v>
+        <v>9451810</v>
       </c>
       <c r="O28">
         <f ca="1"/>
-        <v>7918705</v>
+        <v>12110093</v>
       </c>
       <c r="Q28">
         <f ca="1"/>
-        <v>3520437</v>
+        <v>4260677</v>
       </c>
       <c r="R28">
         <f ca="1"/>
-        <v>3348793</v>
+        <v>4688313</v>
       </c>
       <c r="T28">
         <f ca="1"/>
-        <v>16455876</v>
+        <v>21561903</v>
       </c>
       <c r="U28">
         <f ca="1"/>
-        <v>6869230</v>
+        <v>8948990</v>
       </c>
       <c r="W28">
         <f ca="1"/>
-        <v>9586646</v>
+        <v>12612913</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4533,79 +4536,79 @@
       </c>
       <c r="B29">
         <f ca="1"/>
-        <v>16441448</v>
+        <v>16531166</v>
       </c>
       <c r="C29">
         <f ca="1"/>
-        <v>4199985</v>
+        <v>6592348</v>
       </c>
       <c r="D29">
         <f ca="1"/>
-        <v>8237748</v>
+        <v>17956913</v>
       </c>
       <c r="E29">
         <f ca="1"/>
-        <v>6968982</v>
+        <v>2237031</v>
       </c>
       <c r="F29">
         <f ca="1"/>
-        <v>39774337</v>
+        <v>50157671</v>
       </c>
       <c r="G29">
         <f ca="1"/>
-        <v>2540800</v>
+        <v>4240051</v>
       </c>
       <c r="H29">
         <f ca="1"/>
-        <v>793916</v>
+        <v>1332927</v>
       </c>
       <c r="I29">
         <f ca="1"/>
-        <v>633055</v>
+        <v>1168381</v>
       </c>
       <c r="J29">
         <f ca="1"/>
-        <v>3357039</v>
+        <v>3514324</v>
       </c>
       <c r="K29">
         <f ca="1"/>
-        <v>2154022</v>
+        <v>1157881</v>
       </c>
       <c r="L29">
         <f ca="1"/>
-        <v>5714591</v>
+        <v>7810826</v>
       </c>
       <c r="M29">
         <f ca="1"/>
-        <v>617095</v>
+        <v>812806</v>
       </c>
       <c r="N29">
         <f ca="1"/>
-        <v>7169633</v>
+        <v>8663492</v>
       </c>
       <c r="O29">
         <f ca="1"/>
-        <v>8463027</v>
+        <v>10879544</v>
       </c>
       <c r="Q29">
         <f ca="1"/>
-        <v>3469016</v>
+        <v>3586757</v>
       </c>
       <c r="R29">
         <f ca="1"/>
-        <v>3165843</v>
+        <v>4311816</v>
       </c>
       <c r="T29">
         <f ca="1"/>
-        <v>15632660</v>
+        <v>19543036</v>
       </c>
       <c r="U29">
         <f ca="1"/>
-        <v>6634859</v>
+        <v>7898573</v>
       </c>
       <c r="W29">
         <f ca="1"/>
-        <v>8997801</v>
+        <v>11644463</v>
       </c>
     </row>
   </sheetData>
@@ -5720,10 +5723,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5738,10 +5741,11 @@
     <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="26" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="141" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="141" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="141" t="s">
         <v>0</v>
       </c>
@@ -5775,8 +5779,11 @@
       <c r="K1" s="141" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L1" s="141" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="b">
         <v>0</v>
       </c>
@@ -5810,21 +5817,24 @@
       <c r="K2" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="L2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="5" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9430,7 +9440,7 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -9855,11 +9865,11 @@
       </c>
       <c r="I5" s="16">
         <f ca="1">SIMS_E!W14</f>
-        <v>12413375.5</v>
+        <v>13555723</v>
       </c>
       <c r="J5" s="17">
         <f ca="1">SIMS_E!W15</f>
-        <v>0.43</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="16" x14ac:dyDescent="0.2">
@@ -9905,15 +9915,15 @@
       <c r="F9" s="11"/>
       <c r="H9" s="18">
         <f ca="1">I5* (1 - 0.524417 * J5 / 1.645006)</f>
-        <v>10711735.743050236</v>
+        <v>11092482.497874251</v>
       </c>
       <c r="I9" s="18">
         <f ca="1">I5 * (1-I12)</f>
-        <v>11420305.460000001</v>
+        <v>12471265.16</v>
       </c>
       <c r="J9" s="18">
         <f ca="1">I5* ( 1 - 2/44)</f>
-        <v>11849131.15909091</v>
+        <v>12939553.772727273</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="16" x14ac:dyDescent="0.2">
@@ -10457,31 +10467,31 @@
       </c>
       <c r="B14" s="119">
         <f ca="1">MEDIAN(_xlfn.ANCHORARRAY(B20))</f>
-        <v>0.46650000000000003</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="C14" s="58">
         <f t="shared" ref="C14:P14" ca="1" si="2">MEDIAN(_xlfn.ANCHORARRAY(C20))</f>
-        <v>273.37700000000001</v>
+        <v>281.64400000000001</v>
       </c>
       <c r="D14" s="59">
         <f t="shared" ca="1" si="2"/>
-        <v>171.80500000000001</v>
+        <v>205.93599999999998</v>
       </c>
       <c r="E14" s="59">
         <f t="shared" ca="1" si="2"/>
-        <v>0.32700000000000001</v>
+        <v>0.34450000000000003</v>
       </c>
       <c r="F14" s="59">
         <f t="shared" ca="1" si="2"/>
-        <v>0.39150000000000001</v>
+        <v>0.40900000000000003</v>
       </c>
       <c r="G14" s="59">
         <f t="shared" ca="1" si="2"/>
-        <v>0.74649999999999994</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="H14" s="59">
         <f t="shared" ca="1" si="2"/>
-        <v>0.78200000000000003</v>
+        <v>0.81</v>
       </c>
       <c r="I14" s="60">
         <f t="shared" ca="1" si="2"/>
@@ -10489,27 +10499,27 @@
       </c>
       <c r="J14" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>90.774000000000001</v>
+        <v>98.617500000000007</v>
       </c>
       <c r="K14" s="59">
         <f t="shared" ca="1" si="2"/>
-        <v>72.254999999999995</v>
+        <v>82.584499999999991</v>
       </c>
       <c r="L14" s="59">
         <f t="shared" ca="1" si="2"/>
-        <v>173.57549999999998</v>
+        <v>177.10249999999999</v>
       </c>
       <c r="M14" s="59">
         <f t="shared" ca="1" si="2"/>
-        <v>114.66200000000001</v>
+        <v>136.60649999999998</v>
       </c>
       <c r="N14" s="59">
         <f t="shared" ca="1" si="2"/>
-        <v>139.429</v>
+        <v>114.4765</v>
       </c>
       <c r="O14" s="59">
         <f t="shared" ca="1" si="2"/>
-        <v>98.753999999999991</v>
+        <v>111.164</v>
       </c>
       <c r="P14" s="60">
         <f t="shared" ca="1" si="2"/>
@@ -10525,31 +10535,31 @@
       </c>
       <c r="B15" s="61">
         <f t="shared" ref="B15" ca="1" si="3">ROUND(B16/B14,2)</f>
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C15" s="62">
         <f t="shared" ref="C15:P15" ca="1" si="4">ROUND(C16/C14,2)</f>
-        <v>0.23</v>
+        <v>0.35</v>
       </c>
       <c r="D15" s="63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.37</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E15" s="63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.14000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="F15" s="63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.11</v>
+        <v>0.05</v>
       </c>
       <c r="G15" s="63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="H15" s="63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="I15" s="64" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -10557,27 +10567,27 @@
       </c>
       <c r="J15" s="62">
         <f t="shared" ca="1" si="4"/>
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="K15" s="63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.34</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L15" s="63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.27</v>
+        <v>0.35</v>
       </c>
       <c r="M15" s="63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="N15" s="63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.26</v>
+        <v>0.35</v>
       </c>
       <c r="O15" s="63">
         <f t="shared" ca="1" si="4"/>
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
       <c r="P15" s="64" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -10592,31 +10602,31 @@
       </c>
       <c r="B16" s="65">
         <f t="shared" ref="B16" ca="1" si="5">(B18-B17)/2</f>
-        <v>1.999999999999999E-2</v>
+        <v>1.4999999999999986E-2</v>
       </c>
       <c r="C16" s="66">
         <f t="shared" ref="C16:P16" ca="1" si="6">(C18-C17)/2</f>
-        <v>63.24499999999999</v>
+        <v>97.86999999999999</v>
       </c>
       <c r="D16" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>64.314999999999984</v>
+        <v>57.230000000000004</v>
       </c>
       <c r="E16" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>4.5000000000000012E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F16" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>4.5000000000000012E-2</v>
+        <v>1.999999999999999E-2</v>
       </c>
       <c r="G16" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>0.23000000000000004</v>
+        <v>0.13499999999999995</v>
       </c>
       <c r="H16" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>0.15999999999999998</v>
+        <v>0.17000000000000004</v>
       </c>
       <c r="I16" s="68">
         <f t="shared" ca="1" si="6"/>
@@ -10624,27 +10634,27 @@
       </c>
       <c r="J16" s="66">
         <f t="shared" ca="1" si="6"/>
-        <v>28.93</v>
+        <v>30.99</v>
       </c>
       <c r="K16" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>24.715</v>
+        <v>23.364999999999998</v>
       </c>
       <c r="L16" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>46.834999999999994</v>
+        <v>62.440000000000005</v>
       </c>
       <c r="M16" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>37.645000000000003</v>
+        <v>34.170000000000009</v>
       </c>
       <c r="N16" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>36.82</v>
+        <v>39.585000000000001</v>
       </c>
       <c r="O16" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>41.755000000000003</v>
+        <v>43.865000000000002</v>
       </c>
       <c r="P16" s="68">
         <f t="shared" ca="1" si="6"/>
@@ -10659,31 +10669,31 @@
       </c>
       <c r="B17" s="120">
         <f t="shared" ref="B17:P17" ca="1" si="7">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(B20),ci_alpha/2),2)</f>
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="C17" s="66">
         <f t="shared" ca="1" si="7"/>
-        <v>233.71</v>
+        <v>146.04</v>
       </c>
       <c r="D17" s="67">
         <f t="shared" ca="1" si="7"/>
-        <v>152.71</v>
+        <v>148.72</v>
       </c>
       <c r="E17" s="67">
         <f t="shared" ca="1" si="7"/>
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="F17" s="67">
         <f t="shared" ca="1" si="7"/>
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="G17" s="67">
         <f t="shared" ca="1" si="7"/>
-        <v>0.6</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H17" s="67">
         <f t="shared" ca="1" si="7"/>
-        <v>0.62</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I17" s="68">
         <f t="shared" ca="1" si="7"/>
@@ -10691,27 +10701,27 @@
       </c>
       <c r="J17" s="66">
         <f t="shared" ca="1" si="7"/>
-        <v>71.17</v>
+        <v>50.65</v>
       </c>
       <c r="K17" s="67">
         <f t="shared" ca="1" si="7"/>
-        <v>59.12</v>
+        <v>59.68</v>
       </c>
       <c r="L17" s="67">
         <f t="shared" ca="1" si="7"/>
-        <v>137.21</v>
+        <v>92.83</v>
       </c>
       <c r="M17" s="67">
         <f t="shared" ca="1" si="7"/>
-        <v>101.89</v>
+        <v>100.77</v>
       </c>
       <c r="N17" s="67">
         <f t="shared" ca="1" si="7"/>
-        <v>94.21</v>
+        <v>67.260000000000005</v>
       </c>
       <c r="O17" s="67">
         <f t="shared" ca="1" si="7"/>
-        <v>69.7</v>
+        <v>63.42</v>
       </c>
       <c r="P17" s="68">
         <f t="shared" ca="1" si="7"/>
@@ -10730,27 +10740,27 @@
       </c>
       <c r="C18" s="66">
         <f t="shared" ca="1" si="8"/>
-        <v>360.2</v>
+        <v>341.78</v>
       </c>
       <c r="D18" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>281.33999999999997</v>
+        <v>263.18</v>
       </c>
       <c r="E18" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
       <c r="F18" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="G18" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>1.06</v>
+        <v>0.83</v>
       </c>
       <c r="H18" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>0.94</v>
+        <v>0.92</v>
       </c>
       <c r="I18" s="68">
         <f t="shared" ca="1" si="8"/>
@@ -10758,27 +10768,27 @@
       </c>
       <c r="J18" s="66">
         <f t="shared" ca="1" si="8"/>
-        <v>129.03</v>
+        <v>112.63</v>
       </c>
       <c r="K18" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>108.55</v>
+        <v>106.41</v>
       </c>
       <c r="L18" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>230.88</v>
+        <v>217.71</v>
       </c>
       <c r="M18" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>177.18</v>
+        <v>169.11</v>
       </c>
       <c r="N18" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>167.85</v>
+        <v>146.43</v>
       </c>
       <c r="O18" s="67">
         <f t="shared" ca="1" si="8"/>
-        <v>153.21</v>
+        <v>151.15</v>
       </c>
       <c r="P18" s="68">
         <f t="shared" ca="1" si="8"/>
@@ -10799,17 +10809,17 @@
       <c r="I19" s="56"/>
       <c r="J19" s="69">
         <f ca="1">ROUND(C20*E20, 3)</f>
-        <v>108.465</v>
+        <v>103.562</v>
       </c>
       <c r="K19" s="54"/>
       <c r="L19" s="70">
         <f ca="1">ROUND(C20 * (1  + E20) * $B20,3)</f>
-        <v>179.774</v>
+        <v>187.858</v>
       </c>
       <c r="M19" s="70"/>
       <c r="N19" s="70">
         <f ca="1">ROUND(L20*G20, 3)</f>
-        <v>132.31399999999999</v>
+        <v>150.85</v>
       </c>
       <c r="O19" s="54"/>
       <c r="P19" s="56"/>
@@ -10821,31 +10831,31 @@
       </c>
       <c r="B20" s="72" cm="1">
         <f t="array" aca="1" ref="B20:B29" ca="1">IF(B12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),B6,B7),3),_xlfn.SEQUENCE(n_iter, 1, B6, 0))</f>
-        <v>0.45900000000000002</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="C20" s="72" cm="1">
         <f t="array" aca="1" ref="C20:C29" ca="1">IF(C12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),C6,C7),3),_xlfn.SEQUENCE(n_iter, 1, C6, 0))</f>
-        <v>283.19900000000001</v>
+        <v>282.18400000000003</v>
       </c>
       <c r="D20" s="72" cm="1">
         <f t="array" aca="1" ref="D20:D29" ca="1">IF(D12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),D6,D7),3),_xlfn.SEQUENCE(n_iter, 1, D6, 0))</f>
-        <v>172.78800000000001</v>
+        <v>184.876</v>
       </c>
       <c r="E20" s="72" cm="1">
         <f t="array" aca="1" ref="E20:E29" ca="1">IF(E12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),E6,E7),3),_xlfn.SEQUENCE(n_iter, 1, E6, 0))</f>
-        <v>0.38300000000000001</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="F20" s="72" cm="1">
         <f t="array" aca="1" ref="F20:F29" ca="1">IF(F12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),F6,F7),3),_xlfn.SEQUENCE(n_iter, 1, F6, 0))</f>
-        <v>0.42299999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="G20" s="72" cm="1">
         <f t="array" aca="1" ref="G20:G29" ca="1">IF(G12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),G6,G7),3),_xlfn.SEQUENCE(n_iter, 1, G6, 0))</f>
-        <v>0.73599999999999999</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="H20" s="72" cm="1">
         <f t="array" aca="1" ref="H20:H29" ca="1">IF(H12=1, ROUND(BETAINV(_xlfn.RANDARRAY(n_iter, 1),H9,H10),3),_xlfn.SEQUENCE(n_iter, 1, H6, 0))</f>
-        <v>0.69699999999999995</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="I20" s="72" cm="1">
         <f t="array" aca="1" ref="I20:I29" ca="1">IF(I12=1, ROUND(NORMINV(_xlfn.RANDARRAY(n_iter, 1),I6,I7),3),_xlfn.SEQUENCE(n_iter, 1, I6, 0))</f>
@@ -10853,27 +10863,27 @@
       </c>
       <c r="J20" s="121" cm="1">
         <f t="array" aca="1" ref="J20:J29" ca="1">ROUND(_xlfn.ANCHORARRAY(C20) *_xlfn.ANCHORARRAY( E20), 3)</f>
-        <v>108.465</v>
+        <v>103.562</v>
       </c>
       <c r="K20" s="121" cm="1">
         <f t="array" aca="1" ref="K20:K29" ca="1">ROUND(_xlfn.ANCHORARRAY(D20) *_xlfn.ANCHORARRAY( F20), 3)</f>
-        <v>73.088999999999999</v>
+        <v>72.656000000000006</v>
       </c>
       <c r="L20" s="121" cm="1">
         <f t="array" aca="1" ref="L20:L29" ca="1">ROUND(_xlfn.ANCHORARRAY(C20) * (1 +_xlfn.ANCHORARRAY( E20)) *_xlfn.ANCHORARRAY( $B20), 3)</f>
-        <v>179.774</v>
+        <v>187.858</v>
       </c>
       <c r="M20" s="121" cm="1">
         <f t="array" aca="1" ref="M20:M29" ca="1">ROUND(_xlfn.ANCHORARRAY(D20) * (1 +_xlfn.ANCHORARRAY( F20)) *_xlfn.ANCHORARRAY( $B20), 3)</f>
-        <v>112.858</v>
+        <v>125.41800000000001</v>
       </c>
       <c r="N20" s="121" cm="1">
         <f t="array" aca="1" ref="N20:N29" ca="1">ROUND(_xlfn.ANCHORARRAY(L20) *_xlfn.ANCHORARRAY( G20), 3)</f>
-        <v>132.31399999999999</v>
+        <v>150.85</v>
       </c>
       <c r="O20" s="121" cm="1">
         <f t="array" aca="1" ref="O20:O29" ca="1">ROUND(_xlfn.ANCHORARRAY(M20) *_xlfn.ANCHORARRAY( H20), 3)</f>
-        <v>78.662000000000006</v>
+        <v>89.674000000000007</v>
       </c>
       <c r="P20" s="122" cm="1">
         <f t="array" aca="1" ref="P20:P29" ca="1">_xlfn.ANCHORARRAY(I20)</f>
@@ -10887,31 +10897,31 @@
       </c>
       <c r="B21">
         <f ca="1"/>
-        <v>0.46700000000000003</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="C21">
         <f ca="1"/>
-        <v>381.45299999999997</v>
+        <v>281.10399999999998</v>
       </c>
       <c r="D21">
         <f ca="1"/>
-        <v>259.91699999999997</v>
+        <v>261.017</v>
       </c>
       <c r="E21">
         <f ca="1"/>
-        <v>0.377</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="F21">
         <f ca="1"/>
-        <v>0.36799999999999999</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="G21">
         <f ca="1"/>
-        <v>0.61599999999999999</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="H21">
         <f ca="1"/>
-        <v>0.81499999999999995</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="I21">
         <f ca="1"/>
@@ -10919,27 +10929,27 @@
       </c>
       <c r="J21">
         <f ca="1"/>
-        <v>143.80799999999999</v>
+        <v>99.792000000000002</v>
       </c>
       <c r="K21">
         <f ca="1"/>
-        <v>95.649000000000001</v>
+        <v>108.06100000000001</v>
       </c>
       <c r="L21">
         <f ca="1"/>
-        <v>245.297</v>
+        <v>176.35499999999999</v>
       </c>
       <c r="M21">
         <f ca="1"/>
-        <v>166.05</v>
+        <v>170.88300000000001</v>
       </c>
       <c r="N21">
         <f ca="1"/>
-        <v>151.10300000000001</v>
+        <v>113.925</v>
       </c>
       <c r="O21">
         <f ca="1"/>
-        <v>135.33099999999999</v>
+        <v>155.845</v>
       </c>
       <c r="P21">
         <f ca="1"/>
@@ -10952,31 +10962,31 @@
       </c>
       <c r="B22">
         <f ca="1"/>
-        <v>0.44500000000000001</v>
+        <v>0.47</v>
       </c>
       <c r="C22">
         <f ca="1"/>
-        <v>253.39500000000001</v>
+        <v>328.07299999999998</v>
       </c>
       <c r="D22">
         <f ca="1"/>
-        <v>170.822</v>
+        <v>206.78299999999999</v>
       </c>
       <c r="E22">
         <f ca="1"/>
-        <v>0.29699999999999999</v>
+        <v>0.34899999999999998</v>
       </c>
       <c r="F22">
         <f ca="1"/>
-        <v>0.38100000000000001</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="G22">
         <f ca="1"/>
-        <v>1.002</v>
+        <v>0.55300000000000005</v>
       </c>
       <c r="H22">
         <f ca="1"/>
-        <v>0.93600000000000005</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="I22">
         <f ca="1"/>
@@ -10984,27 +10994,27 @@
       </c>
       <c r="J22">
         <f ca="1"/>
-        <v>75.257999999999996</v>
+        <v>114.497</v>
       </c>
       <c r="K22">
         <f ca="1"/>
-        <v>65.082999999999998</v>
+        <v>83.953999999999994</v>
       </c>
       <c r="L22">
         <f ca="1"/>
-        <v>146.251</v>
+        <v>208.00800000000001</v>
       </c>
       <c r="M22">
         <f ca="1"/>
-        <v>104.97799999999999</v>
+        <v>136.64599999999999</v>
       </c>
       <c r="N22">
         <f ca="1"/>
-        <v>146.54400000000001</v>
+        <v>115.02800000000001</v>
       </c>
       <c r="O22">
         <f ca="1"/>
-        <v>98.259</v>
+        <v>111.503</v>
       </c>
       <c r="P22">
         <f ca="1"/>
@@ -11017,31 +11027,31 @@
       </c>
       <c r="B23">
         <f ca="1"/>
-        <v>0.46800000000000003</v>
+        <v>0.47</v>
       </c>
       <c r="C23">
         <f ca="1"/>
-        <v>290.33999999999997</v>
+        <v>165.93100000000001</v>
       </c>
       <c r="D23">
         <f ca="1"/>
-        <v>251.63300000000001</v>
+        <v>241.24100000000001</v>
       </c>
       <c r="E23">
         <f ca="1"/>
-        <v>0.33300000000000002</v>
+        <v>0.34</v>
       </c>
       <c r="F23">
         <f ca="1"/>
-        <v>0.34200000000000003</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="G23">
         <f ca="1"/>
-        <v>0.873</v>
+        <v>0.84599999999999997</v>
       </c>
       <c r="H23">
         <f ca="1"/>
-        <v>0.628</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="I23">
         <f ca="1"/>
@@ -11049,27 +11059,27 @@
       </c>
       <c r="J23">
         <f ca="1"/>
-        <v>96.683000000000007</v>
+        <v>56.417000000000002</v>
       </c>
       <c r="K23">
         <f ca="1"/>
-        <v>86.058000000000007</v>
+        <v>99.873999999999995</v>
       </c>
       <c r="L23">
         <f ca="1"/>
-        <v>181.12700000000001</v>
+        <v>104.503</v>
       </c>
       <c r="M23">
         <f ca="1"/>
-        <v>158.04</v>
+        <v>160.32400000000001</v>
       </c>
       <c r="N23">
         <f ca="1"/>
-        <v>158.124</v>
+        <v>88.41</v>
       </c>
       <c r="O23">
         <f ca="1"/>
-        <v>99.248999999999995</v>
+        <v>126.977</v>
       </c>
       <c r="P23">
         <f ca="1"/>
@@ -11082,31 +11092,31 @@
       </c>
       <c r="B24">
         <f ca="1"/>
-        <v>0.47899999999999998</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="C24">
         <f ca="1"/>
-        <v>334.23200000000003</v>
+        <v>349.22699999999998</v>
       </c>
       <c r="D24">
         <f ca="1"/>
-        <v>149.221</v>
+        <v>163.87</v>
       </c>
       <c r="E24">
         <f ca="1"/>
-        <v>0.33200000000000002</v>
+        <v>0.316</v>
       </c>
       <c r="F24">
         <f ca="1"/>
-        <v>0.40500000000000003</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="G24">
         <f ca="1"/>
-        <v>0.75700000000000001</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="H24">
         <f ca="1"/>
-        <v>0.621</v>
+        <v>0.88</v>
       </c>
       <c r="I24">
         <f ca="1"/>
@@ -11114,27 +11124,27 @@
       </c>
       <c r="J24">
         <f ca="1"/>
-        <v>110.965</v>
+        <v>110.35599999999999</v>
       </c>
       <c r="K24">
         <f ca="1"/>
-        <v>60.435000000000002</v>
+        <v>69.153000000000006</v>
       </c>
       <c r="L24">
         <f ca="1"/>
-        <v>213.249</v>
+        <v>225.655</v>
       </c>
       <c r="M24">
         <f ca="1"/>
-        <v>100.425</v>
+        <v>114.414</v>
       </c>
       <c r="N24">
         <f ca="1"/>
-        <v>161.429</v>
+        <v>128.172</v>
       </c>
       <c r="O24">
         <f ca="1"/>
-        <v>62.363999999999997</v>
+        <v>100.684</v>
       </c>
       <c r="P24">
         <f ca="1"/>
@@ -11147,31 +11157,31 @@
       </c>
       <c r="B25">
         <f ca="1"/>
-        <v>0.48399999999999999</v>
+        <v>0.47899999999999998</v>
       </c>
       <c r="C25">
         <f ca="1"/>
-        <v>263.55500000000001</v>
+        <v>186.12799999999999</v>
       </c>
       <c r="D25">
         <f ca="1"/>
-        <v>170.29900000000001</v>
+        <v>176.761</v>
       </c>
       <c r="E25">
         <f ca="1"/>
-        <v>0.32200000000000001</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="F25">
         <f ca="1"/>
-        <v>0.41299999999999998</v>
+        <v>0.41199999999999998</v>
       </c>
       <c r="G25">
         <f ca="1"/>
-        <v>0.58099999999999996</v>
+        <v>0.61</v>
       </c>
       <c r="H25">
         <f ca="1"/>
-        <v>0.94</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="I25">
         <f ca="1"/>
@@ -11179,27 +11189,27 @@
       </c>
       <c r="J25">
         <f ca="1"/>
-        <v>84.864999999999995</v>
+        <v>60.677999999999997</v>
       </c>
       <c r="K25">
         <f ca="1"/>
-        <v>70.332999999999998</v>
+        <v>72.825999999999993</v>
       </c>
       <c r="L25">
         <f ca="1"/>
-        <v>168.63499999999999</v>
+        <v>118.22</v>
       </c>
       <c r="M25">
         <f ca="1"/>
-        <v>116.46599999999999</v>
+        <v>119.55200000000001</v>
       </c>
       <c r="N25">
         <f ca="1"/>
-        <v>97.977000000000004</v>
+        <v>72.114000000000004</v>
       </c>
       <c r="O25">
         <f ca="1"/>
-        <v>109.47799999999999</v>
+        <v>110.825</v>
       </c>
       <c r="P25">
         <f ca="1"/>
@@ -11212,31 +11222,31 @@
       </c>
       <c r="B26">
         <f ca="1"/>
-        <v>0.45100000000000001</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="C26">
         <f ca="1"/>
-        <v>263.13600000000002</v>
+        <v>332.685</v>
       </c>
       <c r="D26">
         <f ca="1"/>
-        <v>298.875</v>
+        <v>205.089</v>
       </c>
       <c r="E26">
         <f ca="1"/>
-        <v>0.32</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="F26">
         <f ca="1"/>
-        <v>0.38200000000000001</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="G26">
         <f ca="1"/>
-        <v>1.105</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="H26">
         <f ca="1"/>
-        <v>0.90100000000000002</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="I26">
         <f ca="1"/>
@@ -11244,27 +11254,27 @@
       </c>
       <c r="J26">
         <f ca="1"/>
-        <v>84.203999999999994</v>
+        <v>101.46899999999999</v>
       </c>
       <c r="K26">
         <f ca="1"/>
-        <v>114.17</v>
+        <v>81.215000000000003</v>
       </c>
       <c r="L26">
         <f ca="1"/>
-        <v>156.65</v>
+        <v>207.09100000000001</v>
       </c>
       <c r="M26">
         <f ca="1"/>
-        <v>186.28299999999999</v>
+        <v>136.56700000000001</v>
       </c>
       <c r="N26">
         <f ca="1"/>
-        <v>173.09800000000001</v>
+        <v>141.029</v>
       </c>
       <c r="O26">
         <f ca="1"/>
-        <v>167.84100000000001</v>
+        <v>97.236000000000004</v>
       </c>
       <c r="P26">
         <f ca="1"/>
@@ -11277,31 +11287,31 @@
       </c>
       <c r="B27">
         <f ca="1"/>
-        <v>0.46600000000000003</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="C27">
         <f ca="1"/>
-        <v>286.09500000000003</v>
+        <v>129.75800000000001</v>
       </c>
       <c r="D27">
         <f ca="1"/>
-        <v>253.572</v>
+        <v>230.589</v>
       </c>
       <c r="E27">
         <f ca="1"/>
-        <v>0.33900000000000002</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="F27">
         <f ca="1"/>
-        <v>0.40100000000000002</v>
+        <v>0.433</v>
       </c>
       <c r="G27">
         <f ca="1"/>
-        <v>0.64</v>
+        <v>0.76</v>
       </c>
       <c r="H27">
         <f ca="1"/>
-        <v>0.749</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="I27">
         <f ca="1"/>
@@ -11309,27 +11319,27 @@
       </c>
       <c r="J27">
         <f ca="1"/>
-        <v>96.986000000000004</v>
+        <v>45.933999999999997</v>
       </c>
       <c r="K27">
         <f ca="1"/>
-        <v>101.682</v>
+        <v>99.844999999999999</v>
       </c>
       <c r="L27">
         <f ca="1"/>
-        <v>178.51599999999999</v>
+        <v>83.278000000000006</v>
       </c>
       <c r="M27">
         <f ca="1"/>
-        <v>165.54900000000001</v>
+        <v>156.626</v>
       </c>
       <c r="N27">
         <f ca="1"/>
-        <v>114.25</v>
+        <v>63.290999999999997</v>
       </c>
       <c r="O27">
         <f ca="1"/>
-        <v>123.996</v>
+        <v>125.92700000000001</v>
       </c>
       <c r="P27">
         <f ca="1"/>
@@ -11342,31 +11352,31 @@
       </c>
       <c r="B28">
         <f ca="1"/>
-        <v>0.45400000000000001</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C28">
         <f ca="1"/>
-        <v>217.6</v>
+        <v>266.96699999999998</v>
       </c>
       <c r="D28">
         <f ca="1"/>
-        <v>156.96899999999999</v>
+        <v>264.94799999999998</v>
       </c>
       <c r="E28">
         <f ca="1"/>
-        <v>0.314</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="F28">
         <f ca="1"/>
-        <v>0.45500000000000002</v>
+        <v>0.39400000000000002</v>
       </c>
       <c r="G28">
         <f ca="1"/>
-        <v>0.70199999999999996</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="H28">
         <f ca="1"/>
-        <v>0.93</v>
+        <v>0.871</v>
       </c>
       <c r="I28">
         <f ca="1"/>
@@ -11374,27 +11384,27 @@
       </c>
       <c r="J28">
         <f ca="1"/>
-        <v>68.325999999999993</v>
+        <v>97.442999999999998</v>
       </c>
       <c r="K28">
         <f ca="1"/>
-        <v>71.421000000000006</v>
+        <v>104.39</v>
       </c>
       <c r="L28">
         <f ca="1"/>
-        <v>129.81100000000001</v>
+        <v>164.71299999999999</v>
       </c>
       <c r="M28">
         <f ca="1"/>
-        <v>103.68899999999999</v>
+        <v>166.941</v>
       </c>
       <c r="N28">
         <f ca="1"/>
-        <v>91.126999999999995</v>
+        <v>111.511</v>
       </c>
       <c r="O28">
         <f ca="1"/>
-        <v>96.430999999999997</v>
+        <v>145.40600000000001</v>
       </c>
       <c r="P28">
         <f ca="1"/>
@@ -11407,31 +11417,31 @@
       </c>
       <c r="B29">
         <f ca="1"/>
-        <v>0.49099999999999999</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="C29">
         <f ca="1"/>
-        <v>259.18</v>
+        <v>287.63299999999998</v>
       </c>
       <c r="D29">
         <f ca="1"/>
-        <v>163.95099999999999</v>
+        <v>136.31800000000001</v>
       </c>
       <c r="E29">
         <f ca="1"/>
-        <v>0.28799999999999998</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="F29">
         <f ca="1"/>
-        <v>0.35399999999999998</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="G29">
         <f ca="1"/>
-        <v>0.79400000000000004</v>
+        <v>0.746</v>
       </c>
       <c r="H29">
         <f ca="1"/>
-        <v>0.73699999999999999</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="I29">
         <f ca="1"/>
@@ -11439,27 +11449,27 @@
       </c>
       <c r="J29">
         <f ca="1"/>
-        <v>74.644000000000005</v>
+        <v>86.001999999999995</v>
       </c>
       <c r="K29">
         <f ca="1"/>
-        <v>58.039000000000001</v>
+        <v>51.936999999999998</v>
       </c>
       <c r="L29">
         <f ca="1"/>
-        <v>163.90799999999999</v>
+        <v>177.85</v>
       </c>
       <c r="M29">
         <f ca="1"/>
-        <v>108.997</v>
+        <v>89.608999999999995</v>
       </c>
       <c r="N29">
         <f ca="1"/>
-        <v>130.143</v>
+        <v>132.67599999999999</v>
       </c>
       <c r="O29">
         <f ca="1"/>
-        <v>80.331000000000003</v>
+        <v>41.936999999999998</v>
       </c>
       <c r="P29">
         <f ca="1"/>
@@ -11804,51 +11814,51 @@
       </c>
       <c r="B14" s="58">
         <f t="shared" ref="B14:M14" ca="1" si="0">MEDIAN(_xlfn.ANCHORARRAY(B20))</f>
-        <v>636.44349999999997</v>
+        <v>649.37599999999998</v>
       </c>
       <c r="C14" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>420.42750000000001</v>
+        <v>500.89049999999997</v>
       </c>
       <c r="D14" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>511.23950000000002</v>
+        <v>419.74700000000001</v>
       </c>
       <c r="E14" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>362.09800000000001</v>
+        <v>407.601</v>
       </c>
       <c r="F14" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>157.93049999999999</v>
+        <v>182.06450000000001</v>
       </c>
       <c r="G14" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>108.8725</v>
+        <v>102.37700000000001</v>
       </c>
       <c r="H14" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>636.44349999999997</v>
+        <v>649.37599999999998</v>
       </c>
       <c r="I14" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>420.42750000000001</v>
+        <v>500.89049999999997</v>
       </c>
       <c r="J14" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>511.23950000000002</v>
+        <v>419.74700000000001</v>
       </c>
       <c r="K14" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>362.09800000000001</v>
+        <v>407.601</v>
       </c>
       <c r="L14" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>157.93049999999999</v>
+        <v>182.06450000000001</v>
       </c>
       <c r="M14" s="74">
         <f t="shared" ca="1" si="0"/>
-        <v>108.8725</v>
+        <v>102.37700000000001</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -11857,51 +11867,51 @@
       </c>
       <c r="B15" s="62">
         <f t="shared" ref="B15:M15" ca="1" si="1">ROUND(B16/B14,2)</f>
-        <v>0.27</v>
+        <v>0.35</v>
       </c>
       <c r="C15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="D15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26</v>
+        <v>0.35</v>
       </c>
       <c r="E15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
       <c r="F15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>1.08</v>
+        <v>0.78</v>
       </c>
       <c r="G15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74</v>
+        <v>0.59</v>
       </c>
       <c r="H15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27</v>
+        <v>0.35</v>
       </c>
       <c r="I15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="J15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26</v>
+        <v>0.35</v>
       </c>
       <c r="K15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
       <c r="L15" s="75">
         <f t="shared" ca="1" si="1"/>
-        <v>1.08</v>
+        <v>0.78</v>
       </c>
       <c r="M15" s="76">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -11910,51 +11920,51 @@
       </c>
       <c r="B16" s="58">
         <f t="shared" ref="B16:M16" ca="1" si="2">(B18-B17)/2</f>
-        <v>171.71999999999997</v>
+        <v>228.95499999999998</v>
       </c>
       <c r="C16" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>138.01999999999998</v>
+        <v>125.29000000000002</v>
       </c>
       <c r="D16" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>135.00500000000002</v>
+        <v>145.14499999999998</v>
       </c>
       <c r="E16" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>153.10999999999999</v>
+        <v>160.83500000000004</v>
       </c>
       <c r="F16" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>170.095</v>
+        <v>142.29</v>
       </c>
       <c r="G16" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>81.02000000000001</v>
+        <v>60.39</v>
       </c>
       <c r="H16" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>171.71999999999997</v>
+        <v>228.95499999999998</v>
       </c>
       <c r="I16" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>138.01999999999998</v>
+        <v>125.29000000000002</v>
       </c>
       <c r="J16" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>135.00500000000002</v>
+        <v>145.14499999999998</v>
       </c>
       <c r="K16" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>153.10999999999999</v>
+        <v>160.83500000000004</v>
       </c>
       <c r="L16" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>170.095</v>
+        <v>142.29</v>
       </c>
       <c r="M16" s="74">
         <f t="shared" ca="1" si="2"/>
-        <v>81.02000000000001</v>
+        <v>60.39</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -11963,51 +11973,51 @@
       </c>
       <c r="B17" s="58">
         <f t="shared" ref="B17:M17" ca="1" si="3">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(B20),ci_alpha/2),2)</f>
-        <v>503.1</v>
+        <v>340.37</v>
       </c>
       <c r="C17" s="73">
         <f t="shared" ca="1" si="3"/>
-        <v>373.61</v>
+        <v>369.49</v>
       </c>
       <c r="D17" s="73">
         <f t="shared" ca="1" si="3"/>
-        <v>345.43</v>
+        <v>246.62</v>
       </c>
       <c r="E17" s="73">
         <f t="shared" ca="1" si="3"/>
-        <v>255.56</v>
+        <v>232.54</v>
       </c>
       <c r="F17" s="73">
         <f t="shared" ca="1" si="3"/>
-        <v>-33.65</v>
+        <v>65.430000000000007</v>
       </c>
       <c r="G17" s="73">
         <f t="shared" ca="1" si="3"/>
-        <v>25.08</v>
+        <v>40.25</v>
       </c>
       <c r="H17" s="73">
         <f t="shared" ca="1" si="3"/>
-        <v>503.1</v>
+        <v>340.37</v>
       </c>
       <c r="I17" s="73">
         <f t="shared" ca="1" si="3"/>
-        <v>373.61</v>
+        <v>369.49</v>
       </c>
       <c r="J17" s="73">
         <f t="shared" ca="1" si="3"/>
-        <v>345.43</v>
+        <v>246.62</v>
       </c>
       <c r="K17" s="73">
         <f t="shared" ca="1" si="3"/>
-        <v>255.56</v>
+        <v>232.54</v>
       </c>
       <c r="L17" s="73">
         <f t="shared" ca="1" si="3"/>
-        <v>-33.65</v>
+        <v>65.430000000000007</v>
       </c>
       <c r="M17" s="74">
         <f t="shared" ca="1" si="3"/>
-        <v>25.08</v>
+        <v>40.25</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12016,62 +12026,62 @@
       </c>
       <c r="B18" s="58">
         <f t="shared" ref="B18:M18" ca="1" si="4">ROUND(PERCENTILE(_xlfn.ANCHORARRAY(B20), 1 - ci_alpha / 2), 2)</f>
-        <v>846.54</v>
+        <v>798.28</v>
       </c>
       <c r="C18" s="73">
         <f t="shared" ca="1" si="4"/>
-        <v>649.65</v>
+        <v>620.07000000000005</v>
       </c>
       <c r="D18" s="73">
         <f t="shared" ca="1" si="4"/>
-        <v>615.44000000000005</v>
+        <v>536.91</v>
       </c>
       <c r="E18" s="73">
         <f t="shared" ca="1" si="4"/>
-        <v>561.78</v>
+        <v>554.21</v>
       </c>
       <c r="F18" s="73">
         <f t="shared" ca="1" si="4"/>
-        <v>306.54000000000002</v>
+        <v>350.01</v>
       </c>
       <c r="G18" s="73">
         <f t="shared" ca="1" si="4"/>
-        <v>187.12</v>
+        <v>161.03</v>
       </c>
       <c r="H18" s="73">
         <f t="shared" ca="1" si="4"/>
-        <v>846.54</v>
+        <v>798.28</v>
       </c>
       <c r="I18" s="73">
         <f t="shared" ca="1" si="4"/>
-        <v>649.65</v>
+        <v>620.07000000000005</v>
       </c>
       <c r="J18" s="73">
         <f t="shared" ca="1" si="4"/>
-        <v>615.44000000000005</v>
+        <v>536.91</v>
       </c>
       <c r="K18" s="73">
         <f t="shared" ca="1" si="4"/>
-        <v>561.78</v>
+        <v>554.21</v>
       </c>
       <c r="L18" s="73">
         <f t="shared" ca="1" si="4"/>
-        <v>306.54000000000002</v>
+        <v>350.01</v>
       </c>
       <c r="M18" s="74">
         <f t="shared" ca="1" si="4"/>
-        <v>187.12</v>
+        <v>161.03</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="52"/>
       <c r="B19" s="69">
         <f ca="1">ROUND((SIMS_EF_preparation!L20 - SIMS_EF_preparation!P20) * 44 / 12, 3)</f>
-        <v>659.17100000000005</v>
+        <v>688.81299999999999</v>
       </c>
       <c r="C19" s="127">
         <f ca="1">ROUND((SIMS_EF_preparation!M20 - SIMS_EF_preparation!P20) * 44 / 12, 3)</f>
-        <v>413.81299999999999</v>
+        <v>459.86599999999999</v>
       </c>
       <c r="D19" s="54"/>
       <c r="E19" s="54"/>
@@ -12091,51 +12101,51 @@
       </c>
       <c r="B20" s="72" cm="1">
         <f t="array" aca="1" ref="B20:B29" ca="1">ROUND((_xlfn.XLOOKUP(B$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(B$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>659.17100000000005</v>
+        <v>688.81299999999999</v>
       </c>
       <c r="C20" s="72" cm="1">
         <f t="array" aca="1" ref="C20:C29" ca="1">ROUND((_xlfn.XLOOKUP(C$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(C$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>413.81299999999999</v>
+        <v>459.86599999999999</v>
       </c>
       <c r="D20" s="72" cm="1">
         <f t="array" aca="1" ref="D20:D29" ca="1">ROUND((_xlfn.XLOOKUP(D$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(D$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>485.15100000000001</v>
+        <v>553.11699999999996</v>
       </c>
       <c r="E20" s="72" cm="1">
         <f t="array" aca="1" ref="E20:E29" ca="1">ROUND((_xlfn.XLOOKUP(E$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(E$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>288.42700000000002</v>
+        <v>328.80500000000001</v>
       </c>
       <c r="F20" s="72" cm="1">
         <f t="array" aca="1" ref="F20:F29" ca="1">ROUND((_xlfn.XLOOKUP(F$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(F$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>174.02</v>
+        <v>135.696</v>
       </c>
       <c r="G20" s="72" cm="1">
         <f t="array" aca="1" ref="G20:G29" ca="1">ROUND((_xlfn.XLOOKUP(G$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(G$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>125.38500000000001</v>
+        <v>131.06100000000001</v>
       </c>
       <c r="H20" s="72" cm="1">
         <f t="array" aca="1" ref="H20:H29" ca="1">ROUND((_xlfn.XLOOKUP(H$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(H$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>659.17100000000005</v>
+        <v>688.81299999999999</v>
       </c>
       <c r="I20" s="72" cm="1">
         <f t="array" aca="1" ref="I20:I29" ca="1">ROUND((_xlfn.XLOOKUP(I$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(I$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>413.81299999999999</v>
+        <v>459.86599999999999</v>
       </c>
       <c r="J20" s="72" cm="1">
         <f t="array" aca="1" ref="J20:J29" ca="1">ROUND((_xlfn.XLOOKUP(J$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(J$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>485.15100000000001</v>
+        <v>553.11699999999996</v>
       </c>
       <c r="K20" s="72" cm="1">
         <f t="array" aca="1" ref="K20:K29" ca="1">ROUND((_xlfn.XLOOKUP(K$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(K$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>288.42700000000002</v>
+        <v>328.80500000000001</v>
       </c>
       <c r="L20" s="72" cm="1">
         <f t="array" aca="1" ref="L20:L29" ca="1">ROUND((_xlfn.XLOOKUP(L$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(L$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>174.02</v>
+        <v>135.696</v>
       </c>
       <c r="M20" s="72" cm="1">
         <f t="array" aca="1" ref="M20:M29" ca="1">ROUND((_xlfn.XLOOKUP(M$4, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0) - _xlfn.XLOOKUP(M$5, SIMS_EF_preparation!$L$4:$P$4,_xlfn.ANCHORARRAY( SIMS_EF_preparation!$L20):_xlfn.ANCHORARRAY(SIMS_EF_preparation!$P20),0)) * 44/12, 3)</f>
-        <v>125.38500000000001</v>
+        <v>131.06100000000001</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12144,51 +12154,51 @@
       </c>
       <c r="B21">
         <f ca="1"/>
-        <v>899.42200000000003</v>
+        <v>646.63499999999999</v>
       </c>
       <c r="C21">
         <f ca="1"/>
-        <v>608.85</v>
+        <v>626.57100000000003</v>
       </c>
       <c r="D21">
         <f ca="1"/>
-        <v>554.04399999999998</v>
+        <v>417.72500000000002</v>
       </c>
       <c r="E21">
         <f ca="1"/>
-        <v>496.214</v>
+        <v>571.43200000000002</v>
       </c>
       <c r="F21">
         <f ca="1"/>
-        <v>345.37799999999999</v>
+        <v>228.91</v>
       </c>
       <c r="G21">
         <f ca="1"/>
-        <v>112.636</v>
+        <v>55.139000000000003</v>
       </c>
       <c r="H21">
         <f ca="1"/>
-        <v>899.42200000000003</v>
+        <v>646.63499999999999</v>
       </c>
       <c r="I21">
         <f ca="1"/>
-        <v>608.85</v>
+        <v>626.57100000000003</v>
       </c>
       <c r="J21">
         <f ca="1"/>
-        <v>554.04399999999998</v>
+        <v>417.72500000000002</v>
       </c>
       <c r="K21">
         <f ca="1"/>
-        <v>496.214</v>
+        <v>571.43200000000002</v>
       </c>
       <c r="L21">
         <f ca="1"/>
-        <v>345.37799999999999</v>
+        <v>228.91</v>
       </c>
       <c r="M21">
         <f ca="1"/>
-        <v>112.636</v>
+        <v>55.139000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12197,51 +12207,51 @@
       </c>
       <c r="B22">
         <f ca="1"/>
-        <v>536.25400000000002</v>
+        <v>762.69600000000003</v>
       </c>
       <c r="C22">
         <f ca="1"/>
-        <v>384.91899999999998</v>
+        <v>501.03500000000003</v>
       </c>
       <c r="D22">
         <f ca="1"/>
-        <v>537.32799999999997</v>
+        <v>421.76900000000001</v>
       </c>
       <c r="E22">
         <f ca="1"/>
-        <v>360.28300000000002</v>
+        <v>408.84399999999999</v>
       </c>
       <c r="F22">
         <f ca="1"/>
-        <v>-1.0740000000000001</v>
+        <v>340.92700000000002</v>
       </c>
       <c r="G22">
         <f ca="1"/>
-        <v>24.635999999999999</v>
+        <v>92.191000000000003</v>
       </c>
       <c r="H22">
         <f ca="1"/>
-        <v>536.25400000000002</v>
+        <v>762.69600000000003</v>
       </c>
       <c r="I22">
         <f ca="1"/>
-        <v>384.91899999999998</v>
+        <v>501.03500000000003</v>
       </c>
       <c r="J22">
         <f ca="1"/>
-        <v>537.32799999999997</v>
+        <v>421.76900000000001</v>
       </c>
       <c r="K22">
         <f ca="1"/>
-        <v>360.28300000000002</v>
+        <v>408.84399999999999</v>
       </c>
       <c r="L22">
         <f ca="1"/>
-        <v>-1.0740000000000001</v>
+        <v>340.92700000000002</v>
       </c>
       <c r="M22">
         <f ca="1"/>
-        <v>24.635999999999999</v>
+        <v>92.191000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12250,51 +12260,51 @@
       </c>
       <c r="B23">
         <f ca="1"/>
-        <v>664.13199999999995</v>
+        <v>383.178</v>
       </c>
       <c r="C23">
         <f ca="1"/>
-        <v>579.48</v>
+        <v>587.85500000000002</v>
       </c>
       <c r="D23">
         <f ca="1"/>
-        <v>579.78800000000001</v>
+        <v>324.17</v>
       </c>
       <c r="E23">
         <f ca="1"/>
-        <v>363.91300000000001</v>
+        <v>465.58199999999999</v>
       </c>
       <c r="F23">
         <f ca="1"/>
-        <v>84.343999999999994</v>
+        <v>59.008000000000003</v>
       </c>
       <c r="G23">
         <f ca="1"/>
-        <v>215.56700000000001</v>
+        <v>122.27200000000001</v>
       </c>
       <c r="H23">
         <f ca="1"/>
-        <v>664.13199999999995</v>
+        <v>383.178</v>
       </c>
       <c r="I23">
         <f ca="1"/>
-        <v>579.48</v>
+        <v>587.85500000000002</v>
       </c>
       <c r="J23">
         <f ca="1"/>
-        <v>579.78800000000001</v>
+        <v>324.17</v>
       </c>
       <c r="K23">
         <f ca="1"/>
-        <v>363.91300000000001</v>
+        <v>465.58199999999999</v>
       </c>
       <c r="L23">
         <f ca="1"/>
-        <v>84.343999999999994</v>
+        <v>59.008000000000003</v>
       </c>
       <c r="M23">
         <f ca="1"/>
-        <v>215.56700000000001</v>
+        <v>122.27200000000001</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12303,51 +12313,51 @@
       </c>
       <c r="B24">
         <f ca="1"/>
-        <v>781.91300000000001</v>
+        <v>827.40200000000004</v>
       </c>
       <c r="C24">
         <f ca="1"/>
-        <v>368.22500000000002</v>
+        <v>419.51799999999997</v>
       </c>
       <c r="D24">
         <f ca="1"/>
-        <v>591.90599999999995</v>
+        <v>469.964</v>
       </c>
       <c r="E24">
         <f ca="1"/>
-        <v>228.66800000000001</v>
+        <v>369.17500000000001</v>
       </c>
       <c r="F24">
         <f ca="1"/>
-        <v>190.00700000000001</v>
+        <v>357.43799999999999</v>
       </c>
       <c r="G24">
         <f ca="1"/>
-        <v>139.55699999999999</v>
+        <v>50.343000000000004</v>
       </c>
       <c r="H24">
         <f ca="1"/>
-        <v>781.91300000000001</v>
+        <v>827.40200000000004</v>
       </c>
       <c r="I24">
         <f ca="1"/>
-        <v>368.22500000000002</v>
+        <v>419.51799999999997</v>
       </c>
       <c r="J24">
         <f ca="1"/>
-        <v>591.90599999999995</v>
+        <v>469.964</v>
       </c>
       <c r="K24">
         <f ca="1"/>
-        <v>228.66800000000001</v>
+        <v>369.17500000000001</v>
       </c>
       <c r="L24">
         <f ca="1"/>
-        <v>190.00700000000001</v>
+        <v>357.43799999999999</v>
       </c>
       <c r="M24">
         <f ca="1"/>
-        <v>139.55699999999999</v>
+        <v>50.343000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12356,51 +12366,51 @@
       </c>
       <c r="B25">
         <f ca="1"/>
-        <v>618.32799999999997</v>
+        <v>433.47300000000001</v>
       </c>
       <c r="C25">
         <f ca="1"/>
-        <v>427.04199999999997</v>
+        <v>438.35700000000003</v>
       </c>
       <c r="D25">
         <f ca="1"/>
-        <v>359.24900000000002</v>
+        <v>264.41800000000001</v>
       </c>
       <c r="E25">
         <f ca="1"/>
-        <v>401.41899999999998</v>
+        <v>406.358</v>
       </c>
       <c r="F25">
         <f ca="1"/>
-        <v>259.07900000000001</v>
+        <v>169.05500000000001</v>
       </c>
       <c r="G25">
         <f ca="1"/>
-        <v>25.623000000000001</v>
+        <v>31.998999999999999</v>
       </c>
       <c r="H25">
         <f ca="1"/>
-        <v>618.32799999999997</v>
+        <v>433.47300000000001</v>
       </c>
       <c r="I25">
         <f ca="1"/>
-        <v>427.04199999999997</v>
+        <v>438.35700000000003</v>
       </c>
       <c r="J25">
         <f ca="1"/>
-        <v>359.24900000000002</v>
+        <v>264.41800000000001</v>
       </c>
       <c r="K25">
         <f ca="1"/>
-        <v>401.41899999999998</v>
+        <v>406.358</v>
       </c>
       <c r="L25">
         <f ca="1"/>
-        <v>259.07900000000001</v>
+        <v>169.05500000000001</v>
       </c>
       <c r="M25">
         <f ca="1"/>
-        <v>25.623000000000001</v>
+        <v>31.998999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12409,51 +12419,51 @@
       </c>
       <c r="B26">
         <f ca="1"/>
-        <v>574.38300000000004</v>
+        <v>759.33399999999995</v>
       </c>
       <c r="C26">
         <f ca="1"/>
-        <v>683.03800000000001</v>
+        <v>500.74599999999998</v>
       </c>
       <c r="D26">
         <f ca="1"/>
-        <v>634.69299999999998</v>
+        <v>517.10599999999999</v>
       </c>
       <c r="E26">
         <f ca="1"/>
-        <v>615.41700000000003</v>
+        <v>356.53199999999998</v>
       </c>
       <c r="F26">
         <f ca="1"/>
-        <v>-60.308999999999997</v>
+        <v>242.227</v>
       </c>
       <c r="G26">
         <f ca="1"/>
-        <v>67.620999999999995</v>
+        <v>144.214</v>
       </c>
       <c r="H26">
         <f ca="1"/>
-        <v>574.38300000000004</v>
+        <v>759.33399999999995</v>
       </c>
       <c r="I26">
         <f ca="1"/>
-        <v>683.03800000000001</v>
+        <v>500.74599999999998</v>
       </c>
       <c r="J26">
         <f ca="1"/>
-        <v>634.69299999999998</v>
+        <v>517.10599999999999</v>
       </c>
       <c r="K26">
         <f ca="1"/>
-        <v>615.41700000000003</v>
+        <v>356.53199999999998</v>
       </c>
       <c r="L26">
         <f ca="1"/>
-        <v>-60.308999999999997</v>
+        <v>242.227</v>
       </c>
       <c r="M26">
         <f ca="1"/>
-        <v>67.620999999999995</v>
+        <v>144.214</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12462,51 +12472,51 @@
       </c>
       <c r="B27">
         <f ca="1"/>
-        <v>654.55899999999997</v>
+        <v>305.35300000000001</v>
       </c>
       <c r="C27">
         <f ca="1"/>
-        <v>607.01300000000003</v>
+        <v>574.29499999999996</v>
       </c>
       <c r="D27">
         <f ca="1"/>
-        <v>418.91699999999997</v>
+        <v>232.06700000000001</v>
       </c>
       <c r="E27">
         <f ca="1"/>
-        <v>454.65199999999999</v>
+        <v>461.73200000000003</v>
       </c>
       <c r="F27">
         <f ca="1"/>
-        <v>235.642</v>
+        <v>73.286000000000001</v>
       </c>
       <c r="G27">
         <f ca="1"/>
-        <v>152.36099999999999</v>
+        <v>112.563</v>
       </c>
       <c r="H27">
         <f ca="1"/>
-        <v>654.55899999999997</v>
+        <v>305.35300000000001</v>
       </c>
       <c r="I27">
         <f ca="1"/>
-        <v>607.01300000000003</v>
+        <v>574.29499999999996</v>
       </c>
       <c r="J27">
         <f ca="1"/>
-        <v>418.91699999999997</v>
+        <v>232.06700000000001</v>
       </c>
       <c r="K27">
         <f ca="1"/>
-        <v>454.65199999999999</v>
+        <v>461.73200000000003</v>
       </c>
       <c r="L27">
         <f ca="1"/>
-        <v>235.642</v>
+        <v>73.286000000000001</v>
       </c>
       <c r="M27">
         <f ca="1"/>
-        <v>152.36099999999999</v>
+        <v>112.563</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12515,51 +12525,51 @@
       </c>
       <c r="B28">
         <f ca="1"/>
-        <v>475.97399999999999</v>
+        <v>603.94799999999998</v>
       </c>
       <c r="C28">
         <f ca="1"/>
-        <v>380.19299999999998</v>
+        <v>612.11699999999996</v>
       </c>
       <c r="D28">
         <f ca="1"/>
-        <v>334.13200000000001</v>
+        <v>408.87400000000002</v>
       </c>
       <c r="E28">
         <f ca="1"/>
-        <v>353.58</v>
+        <v>533.15499999999997</v>
       </c>
       <c r="F28">
         <f ca="1"/>
-        <v>141.84100000000001</v>
+        <v>195.07400000000001</v>
       </c>
       <c r="G28">
         <f ca="1"/>
-        <v>26.613</v>
+        <v>78.962000000000003</v>
       </c>
       <c r="H28">
         <f ca="1"/>
-        <v>475.97399999999999</v>
+        <v>603.94799999999998</v>
       </c>
       <c r="I28">
         <f ca="1"/>
-        <v>380.19299999999998</v>
+        <v>612.11699999999996</v>
       </c>
       <c r="J28">
         <f ca="1"/>
-        <v>334.13200000000001</v>
+        <v>408.87400000000002</v>
       </c>
       <c r="K28">
         <f ca="1"/>
-        <v>353.58</v>
+        <v>533.15499999999997</v>
       </c>
       <c r="L28">
         <f ca="1"/>
-        <v>141.84100000000001</v>
+        <v>195.07400000000001</v>
       </c>
       <c r="M28">
         <f ca="1"/>
-        <v>26.613</v>
+        <v>78.962000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12568,51 +12578,51 @@
       </c>
       <c r="B29">
         <f ca="1"/>
-        <v>600.99599999999998</v>
+        <v>652.11699999999996</v>
       </c>
       <c r="C29">
         <f ca="1"/>
-        <v>399.65600000000001</v>
+        <v>328.56599999999997</v>
       </c>
       <c r="D29">
         <f ca="1"/>
-        <v>477.19099999999997</v>
+        <v>486.47899999999998</v>
       </c>
       <c r="E29">
         <f ca="1"/>
-        <v>294.54700000000003</v>
+        <v>153.76900000000001</v>
       </c>
       <c r="F29">
         <f ca="1"/>
-        <v>123.80500000000001</v>
+        <v>165.63800000000001</v>
       </c>
       <c r="G29">
         <f ca="1"/>
-        <v>105.10899999999999</v>
+        <v>174.797</v>
       </c>
       <c r="H29">
         <f ca="1"/>
-        <v>600.99599999999998</v>
+        <v>652.11699999999996</v>
       </c>
       <c r="I29">
         <f ca="1"/>
-        <v>399.65600000000001</v>
+        <v>328.56599999999997</v>
       </c>
       <c r="J29">
         <f ca="1"/>
-        <v>477.19099999999997</v>
+        <v>486.47899999999998</v>
       </c>
       <c r="K29">
         <f ca="1"/>
-        <v>294.54700000000003</v>
+        <v>153.76900000000001</v>
       </c>
       <c r="L29">
         <f ca="1"/>
-        <v>123.80500000000001</v>
+        <v>165.63800000000001</v>
       </c>
       <c r="M29">
         <f ca="1"/>
-        <v>105.10899999999999</v>
+        <v>174.797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>